<commit_message>
changed upload files application and recommendation
</commit_message>
<xml_diff>
--- a/app/assets/files/NAPI 2013 Application Form.xlsx
+++ b/app/assets/files/NAPI 2013 Application Form.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23416"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr checkCompatibility="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="13940" tabRatio="500"/>
+    <workbookView xWindow="-735" yWindow="-21045" windowWidth="20730" windowHeight="11760" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Application" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
@@ -218,9 +218,6 @@
     <t>1 year</t>
   </si>
   <si>
-    <t>Example:  Experience with vacuum systems</t>
-  </si>
-  <si>
     <t>4. Why should you be accepted into this program? (100 words)</t>
   </si>
   <si>
@@ -331,17 +328,31 @@
     </r>
   </si>
   <si>
-    <t>5. Send the PDF files to internship.naist@gmail.com on or before July 19, 2013 11:59 PM (Philippine standard time) with NAPI2013 Application as the subject line of your email.</t>
-  </si>
-  <si>
-    <t>7. Deadline for the recommendation form is on or before July 19, 2013 11:59 PM (Philippine standard time). Please contact your professors/advisers beforehand about your application. Kindly ask them to send the document directly to internship.naist@gmail.com in PDF format.</t>
+    <t>5. Send the PDF files to internship.naist@gmail.com on or before July 19, 2013 23:59 GMT+8 with NAPI2013 Application as the subject line of your email.</t>
+  </si>
+  <si>
+    <t>7. Deadline for the recommendation form is on or before July 19, 2013 23:59 GMT+8. Please contact your professors/advisers beforehand about your application. Kindly ask them to send the document directly to internship.naist@gmail.com in PDF format.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Example:  Experience with vacuum systems </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>(Kindly delete this when filling this part)</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="31" x14ac:knownFonts="1">
+  <fonts count="32" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -502,6 +513,12 @@
       <u/>
       <sz val="10"/>
       <color theme="11"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
   </fonts>
@@ -909,6 +926,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1017,6 +1036,9 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1026,17 +1048,12 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1045,6 +1062,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1370,46 +1392,48 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E116"/>
+  <dimension ref="A1:F132"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22:E24"/>
+    <sheetView tabSelected="1" showWhiteSpace="0" view="pageLayout" workbookViewId="0">
+      <selection activeCell="D66" sqref="D66:E66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14.25" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.25" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="3" width="23" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" customWidth="1"/>
-    <col min="5" max="5" width="9.1640625" customWidth="1"/>
-    <col min="6" max="6" width="2.1640625" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" customWidth="1"/>
+    <col min="6" max="6" width="2.140625" hidden="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A1" s="47" t="s">
+    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-    </row>
-    <row r="3" spans="1:5" ht="13">
-      <c r="A3" s="43" t="s">
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+    </row>
+    <row r="2" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="44"/>
-      <c r="C3" s="44"/>
-      <c r="D3" s="44"/>
-      <c r="E3" s="44"/>
-    </row>
-    <row r="4" spans="1:5" ht="6" customHeight="1">
+      <c r="B3" s="46"/>
+      <c r="C3" s="46"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="46"/>
+    </row>
+    <row r="4" spans="1:5" ht="6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="10"/>
       <c r="B4" s="10"/>
       <c r="C4" s="10"/>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
     </row>
-    <row r="5" spans="1:5" ht="13">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>2</v>
       </c>
@@ -1419,19 +1443,19 @@
       <c r="C5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="59" t="s">
+      <c r="D5" s="61" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="60"/>
-    </row>
-    <row r="6" spans="1:5" ht="30" customHeight="1">
+      <c r="E5" s="57"/>
+    </row>
+    <row r="6" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="11"/>
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
-      <c r="D6" s="23"/>
-      <c r="E6" s="60"/>
-    </row>
-    <row r="7" spans="1:5" ht="13">
+      <c r="D6" s="25"/>
+      <c r="E6" s="57"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>6</v>
       </c>
@@ -1441,130 +1465,130 @@
       <c r="C7" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="23"/>
-      <c r="E7" s="60"/>
-    </row>
-    <row r="8" spans="1:5" ht="30" customHeight="1">
+      <c r="D7" s="25"/>
+      <c r="E7" s="57"/>
+    </row>
+    <row r="8" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="11"/>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
-      <c r="D8" s="23"/>
-      <c r="E8" s="60"/>
-    </row>
-    <row r="9" spans="1:5" ht="13">
-      <c r="A9" s="58" t="s">
+      <c r="D8" s="25"/>
+      <c r="E8" s="57"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="62" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="21"/>
+      <c r="B9" s="23"/>
       <c r="C9" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="23"/>
-      <c r="E9" s="60"/>
-    </row>
-    <row r="10" spans="1:5" ht="30" customHeight="1">
-      <c r="A10" s="57"/>
-      <c r="B10" s="21"/>
+      <c r="D9" s="25"/>
+      <c r="E9" s="57"/>
+    </row>
+    <row r="10" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="60"/>
+      <c r="B10" s="23"/>
       <c r="C10" s="11"/>
-      <c r="D10" s="23"/>
-      <c r="E10" s="60"/>
-    </row>
-    <row r="11" spans="1:5" ht="25" customHeight="1">
+      <c r="D10" s="25"/>
+      <c r="E10" s="57"/>
+    </row>
+    <row r="11" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
     </row>
-    <row r="12" spans="1:5" ht="13">
-      <c r="A12" s="43" t="s">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="45" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="44"/>
-      <c r="C12" s="44"/>
-      <c r="D12" s="44"/>
-      <c r="E12" s="44"/>
-    </row>
-    <row r="13" spans="1:5" ht="6" customHeight="1">
+      <c r="B12" s="46"/>
+      <c r="C12" s="46"/>
+      <c r="D12" s="46"/>
+      <c r="E12" s="46"/>
+    </row>
+    <row r="13" spans="1:5" ht="6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="10"/>
       <c r="B13" s="10"/>
       <c r="C13" s="10"/>
       <c r="D13" s="10"/>
       <c r="E13" s="10"/>
     </row>
-    <row r="14" spans="1:5" ht="30" customHeight="1">
-      <c r="A14" s="54" t="s">
+    <row r="14" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="56" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="21"/>
+      <c r="B14" s="23"/>
       <c r="C14" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="56" t="s">
+      <c r="D14" s="59" t="s">
         <v>14</v>
       </c>
-      <c r="E14" s="60"/>
-    </row>
-    <row r="15" spans="1:5" ht="30" customHeight="1">
-      <c r="A15" s="57"/>
-      <c r="B15" s="21"/>
+      <c r="E14" s="57"/>
+    </row>
+    <row r="15" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="60"/>
+      <c r="B15" s="23"/>
       <c r="C15" s="11"/>
-      <c r="D15" s="49"/>
-      <c r="E15" s="60"/>
-    </row>
-    <row r="16" spans="1:5" ht="13">
-      <c r="A16" s="54" t="s">
+      <c r="D15" s="51"/>
+      <c r="E15" s="57"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="56" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="46"/>
-      <c r="C16" s="21"/>
-      <c r="D16" s="48" t="s">
+      <c r="B16" s="48"/>
+      <c r="C16" s="23"/>
+      <c r="D16" s="50" t="s">
         <v>16</v>
       </c>
-      <c r="E16" s="60"/>
-    </row>
-    <row r="17" spans="1:5" ht="30" customHeight="1">
-      <c r="A17" s="49"/>
-      <c r="B17" s="46"/>
-      <c r="C17" s="21"/>
-      <c r="D17" s="49"/>
-      <c r="E17" s="60"/>
-    </row>
-    <row r="18" spans="1:5" ht="30" customHeight="1">
-      <c r="A18" s="55" t="s">
+      <c r="E16" s="57"/>
+    </row>
+    <row r="17" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="51"/>
+      <c r="B17" s="48"/>
+      <c r="C17" s="23"/>
+      <c r="D17" s="51"/>
+      <c r="E17" s="57"/>
+    </row>
+    <row r="18" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="B18" s="20"/>
-      <c r="C18" s="20"/>
-      <c r="D18" s="20"/>
-      <c r="E18" s="60"/>
-    </row>
-    <row r="19" spans="1:5" ht="30" customHeight="1">
-      <c r="A19" s="49"/>
-      <c r="B19" s="46"/>
-      <c r="C19" s="46"/>
-      <c r="D19" s="46"/>
-      <c r="E19" s="20"/>
-    </row>
-    <row r="20" spans="1:5" ht="13">
-      <c r="A20" s="50" t="s">
+      <c r="B18" s="22"/>
+      <c r="C18" s="22"/>
+      <c r="D18" s="22"/>
+      <c r="E18" s="57"/>
+    </row>
+    <row r="19" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="51"/>
+      <c r="B19" s="48"/>
+      <c r="C19" s="48"/>
+      <c r="D19" s="48"/>
+      <c r="E19" s="22"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="52" t="s">
         <v>17</v>
       </c>
-      <c r="B20" s="20"/>
-      <c r="C20" s="20"/>
-      <c r="D20" s="20"/>
-      <c r="E20" s="21"/>
-    </row>
-    <row r="21" spans="1:5" ht="30" customHeight="1">
-      <c r="A21" s="51" t="s">
-        <v>49</v>
-      </c>
-      <c r="B21" s="52"/>
-      <c r="C21" s="52"/>
-      <c r="D21" s="52"/>
-      <c r="E21" s="53"/>
-    </row>
-    <row r="22" spans="1:5" ht="30" customHeight="1">
+      <c r="B20" s="22"/>
+      <c r="C20" s="22"/>
+      <c r="D20" s="22"/>
+      <c r="E20" s="23"/>
+    </row>
+    <row r="21" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="53" t="s">
+        <v>48</v>
+      </c>
+      <c r="B21" s="54"/>
+      <c r="C21" s="54"/>
+      <c r="D21" s="54"/>
+      <c r="E21" s="55"/>
+    </row>
+    <row r="22" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="8" t="s">
         <v>18</v>
       </c>
@@ -1573,9 +1597,9 @@
       </c>
       <c r="C22" s="7"/>
       <c r="D22" s="7"/>
-      <c r="E22" s="61"/>
-    </row>
-    <row r="23" spans="1:5" ht="30" customHeight="1">
+      <c r="E22" s="19"/>
+    </row>
+    <row r="23" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="8" t="s">
         <v>20</v>
       </c>
@@ -1584,517 +1608,517 @@
       </c>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
-      <c r="E23" s="61"/>
-    </row>
-    <row r="24" spans="1:5" ht="13">
+      <c r="E23" s="19"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="12"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
-      <c r="E24" s="62"/>
-    </row>
-    <row r="25" spans="1:5" ht="25" customHeight="1">
+      <c r="E24" s="20"/>
+    </row>
+    <row r="25" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
     </row>
-    <row r="26" spans="1:5" ht="13">
-      <c r="A26" s="43" t="s">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" s="45" t="s">
         <v>21</v>
       </c>
-      <c r="B26" s="44"/>
-      <c r="C26" s="44"/>
-      <c r="D26" s="44"/>
-      <c r="E26" s="44"/>
-    </row>
-    <row r="27" spans="1:5" ht="4.5" customHeight="1">
+      <c r="B26" s="46"/>
+      <c r="C26" s="46"/>
+      <c r="D26" s="46"/>
+      <c r="E26" s="46"/>
+    </row>
+    <row r="27" spans="1:5" ht="4.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="10"/>
       <c r="B27" s="10"/>
       <c r="C27" s="10"/>
       <c r="D27" s="10"/>
       <c r="E27" s="10"/>
     </row>
-    <row r="28" spans="1:5" ht="13">
-      <c r="A28" s="48" t="s">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" s="50" t="s">
         <v>22</v>
       </c>
-      <c r="B28" s="20"/>
-      <c r="C28" s="20"/>
-      <c r="D28" s="20"/>
-      <c r="E28" s="21"/>
-    </row>
-    <row r="29" spans="1:5" ht="22.5" customHeight="1">
-      <c r="A29" s="24"/>
-      <c r="B29" s="20"/>
-      <c r="C29" s="20"/>
-      <c r="D29" s="20"/>
-      <c r="E29" s="21"/>
-    </row>
-    <row r="30" spans="1:5" ht="13">
-      <c r="A30" s="48" t="s">
+      <c r="B28" s="22"/>
+      <c r="C28" s="22"/>
+      <c r="D28" s="22"/>
+      <c r="E28" s="23"/>
+    </row>
+    <row r="29" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="26"/>
+      <c r="B29" s="22"/>
+      <c r="C29" s="22"/>
+      <c r="D29" s="22"/>
+      <c r="E29" s="23"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" s="50" t="s">
         <v>23</v>
       </c>
-      <c r="B30" s="20"/>
-      <c r="C30" s="20"/>
-      <c r="D30" s="20"/>
-      <c r="E30" s="21"/>
-    </row>
-    <row r="31" spans="1:5" ht="22.5" customHeight="1">
-      <c r="A31" s="24"/>
-      <c r="B31" s="20"/>
-      <c r="C31" s="20"/>
-      <c r="D31" s="20"/>
-      <c r="E31" s="21"/>
-    </row>
-    <row r="32" spans="1:5" ht="13">
-      <c r="A32" s="48" t="s">
+      <c r="B30" s="22"/>
+      <c r="C30" s="22"/>
+      <c r="D30" s="22"/>
+      <c r="E30" s="23"/>
+    </row>
+    <row r="31" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="26"/>
+      <c r="B31" s="22"/>
+      <c r="C31" s="22"/>
+      <c r="D31" s="22"/>
+      <c r="E31" s="23"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" s="50" t="s">
         <v>24</v>
       </c>
-      <c r="B32" s="20"/>
-      <c r="C32" s="20"/>
-      <c r="D32" s="20"/>
-      <c r="E32" s="21"/>
-    </row>
-    <row r="33" spans="1:5" ht="22.5" customHeight="1">
-      <c r="A33" s="24"/>
-      <c r="B33" s="20"/>
-      <c r="C33" s="20"/>
-      <c r="D33" s="20"/>
-      <c r="E33" s="21"/>
-    </row>
-    <row r="34" spans="1:5" ht="15" customHeight="1">
+      <c r="B32" s="22"/>
+      <c r="C32" s="22"/>
+      <c r="D32" s="22"/>
+      <c r="E32" s="23"/>
+    </row>
+    <row r="33" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="26"/>
+      <c r="B33" s="22"/>
+      <c r="C33" s="22"/>
+      <c r="D33" s="22"/>
+      <c r="E33" s="23"/>
+    </row>
+    <row r="34" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
       <c r="E34" s="3"/>
     </row>
-    <row r="35" spans="1:5" ht="12">
-      <c r="A35" s="42" t="s">
+    <row r="35" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A35" s="44" t="s">
         <v>25</v>
       </c>
-      <c r="B35" s="27"/>
-      <c r="C35" s="27"/>
-      <c r="D35" s="27"/>
-      <c r="E35" s="27"/>
-    </row>
-    <row r="36" spans="1:5" ht="22.5" customHeight="1">
+      <c r="B35" s="29"/>
+      <c r="C35" s="29"/>
+      <c r="D35" s="29"/>
+      <c r="E35" s="29"/>
+    </row>
+    <row r="36" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B36" s="43"/>
-      <c r="C36" s="44"/>
-    </row>
-    <row r="37" spans="1:5" ht="22.5" customHeight="1">
+      <c r="B36" s="45"/>
+      <c r="C36" s="46"/>
+    </row>
+    <row r="37" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B37" s="45"/>
-      <c r="C37" s="46"/>
-    </row>
-    <row r="38" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A38" s="47" t="s">
+      <c r="B37" s="47"/>
+      <c r="C37" s="48"/>
+    </row>
+    <row r="38" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="B38" s="27"/>
-      <c r="C38" s="27"/>
-      <c r="D38" s="27"/>
-      <c r="E38" s="27"/>
-    </row>
-    <row r="39" spans="1:5" ht="12">
+      <c r="B38" s="29"/>
+      <c r="C38" s="29"/>
+      <c r="D38" s="29"/>
+      <c r="E38" s="29"/>
+    </row>
+    <row r="39" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A39" s="9"/>
       <c r="B39" s="9"/>
       <c r="C39" s="9"/>
       <c r="D39" s="9"/>
       <c r="E39" s="9"/>
     </row>
-    <row r="40" spans="1:5" ht="30" customHeight="1">
-      <c r="A40" s="25" t="s">
+    <row r="40" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="B40" s="20"/>
-      <c r="C40" s="20"/>
-      <c r="D40" s="20"/>
-      <c r="E40" s="21"/>
-    </row>
-    <row r="41" spans="1:5" ht="12">
-      <c r="A41" s="24"/>
-      <c r="B41" s="20"/>
-      <c r="C41" s="20"/>
-      <c r="D41" s="20"/>
-      <c r="E41" s="21"/>
-    </row>
-    <row r="42" spans="1:5" ht="12">
-      <c r="A42" s="23"/>
-      <c r="B42" s="20"/>
-      <c r="C42" s="20"/>
-      <c r="D42" s="20"/>
-      <c r="E42" s="21"/>
-    </row>
-    <row r="43" spans="1:5" ht="12">
-      <c r="A43" s="23"/>
-      <c r="B43" s="20"/>
-      <c r="C43" s="20"/>
-      <c r="D43" s="20"/>
-      <c r="E43" s="21"/>
-    </row>
-    <row r="44" spans="1:5" s="18" customFormat="1" ht="12">
-      <c r="A44" s="23"/>
-      <c r="B44" s="20"/>
-      <c r="C44" s="20"/>
-      <c r="D44" s="20"/>
-      <c r="E44" s="21"/>
-    </row>
-    <row r="45" spans="1:5" s="18" customFormat="1" ht="12">
-      <c r="A45" s="23"/>
-      <c r="B45" s="20"/>
-      <c r="C45" s="20"/>
-      <c r="D45" s="20"/>
-      <c r="E45" s="21"/>
-    </row>
-    <row r="46" spans="1:5" ht="12">
-      <c r="A46" s="23"/>
-      <c r="B46" s="20"/>
-      <c r="C46" s="20"/>
-      <c r="D46" s="20"/>
-      <c r="E46" s="21"/>
-    </row>
-    <row r="47" spans="1:5" ht="12">
-      <c r="A47" s="23"/>
-      <c r="B47" s="20"/>
-      <c r="C47" s="20"/>
-      <c r="D47" s="20"/>
-      <c r="E47" s="21"/>
-    </row>
-    <row r="48" spans="1:5" ht="12">
-      <c r="A48" s="23"/>
-      <c r="B48" s="20"/>
-      <c r="C48" s="20"/>
-      <c r="D48" s="20"/>
-      <c r="E48" s="21"/>
-    </row>
-    <row r="49" spans="1:5" ht="12">
-      <c r="A49" s="23"/>
-      <c r="B49" s="20"/>
-      <c r="C49" s="20"/>
-      <c r="D49" s="20"/>
-      <c r="E49" s="21"/>
-    </row>
-    <row r="50" spans="1:5" ht="12">
-      <c r="A50" s="23"/>
-      <c r="B50" s="20"/>
-      <c r="C50" s="20"/>
-      <c r="D50" s="20"/>
-      <c r="E50" s="21"/>
-    </row>
-    <row r="51" spans="1:5" ht="30" customHeight="1">
-      <c r="A51" s="19" t="s">
+      <c r="B40" s="22"/>
+      <c r="C40" s="22"/>
+      <c r="D40" s="22"/>
+      <c r="E40" s="23"/>
+    </row>
+    <row r="41" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A41" s="26"/>
+      <c r="B41" s="22"/>
+      <c r="C41" s="22"/>
+      <c r="D41" s="22"/>
+      <c r="E41" s="23"/>
+    </row>
+    <row r="42" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A42" s="25"/>
+      <c r="B42" s="22"/>
+      <c r="C42" s="22"/>
+      <c r="D42" s="22"/>
+      <c r="E42" s="23"/>
+    </row>
+    <row r="43" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A43" s="25"/>
+      <c r="B43" s="22"/>
+      <c r="C43" s="22"/>
+      <c r="D43" s="22"/>
+      <c r="E43" s="23"/>
+    </row>
+    <row r="44" spans="1:5" s="18" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A44" s="25"/>
+      <c r="B44" s="22"/>
+      <c r="C44" s="22"/>
+      <c r="D44" s="22"/>
+      <c r="E44" s="23"/>
+    </row>
+    <row r="45" spans="1:5" s="18" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A45" s="25"/>
+      <c r="B45" s="22"/>
+      <c r="C45" s="22"/>
+      <c r="D45" s="22"/>
+      <c r="E45" s="23"/>
+    </row>
+    <row r="46" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A46" s="25"/>
+      <c r="B46" s="22"/>
+      <c r="C46" s="22"/>
+      <c r="D46" s="22"/>
+      <c r="E46" s="23"/>
+    </row>
+    <row r="47" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A47" s="25"/>
+      <c r="B47" s="22"/>
+      <c r="C47" s="22"/>
+      <c r="D47" s="22"/>
+      <c r="E47" s="23"/>
+    </row>
+    <row r="48" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A48" s="25"/>
+      <c r="B48" s="22"/>
+      <c r="C48" s="22"/>
+      <c r="D48" s="22"/>
+      <c r="E48" s="23"/>
+    </row>
+    <row r="49" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A49" s="25"/>
+      <c r="B49" s="22"/>
+      <c r="C49" s="22"/>
+      <c r="D49" s="22"/>
+      <c r="E49" s="23"/>
+    </row>
+    <row r="50" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A50" s="25"/>
+      <c r="B50" s="22"/>
+      <c r="C50" s="22"/>
+      <c r="D50" s="22"/>
+      <c r="E50" s="23"/>
+    </row>
+    <row r="51" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="B51" s="20"/>
-      <c r="C51" s="20"/>
-      <c r="D51" s="20"/>
-      <c r="E51" s="21"/>
-    </row>
-    <row r="52" spans="1:5" ht="12">
-      <c r="A52" s="24"/>
-      <c r="B52" s="20"/>
-      <c r="C52" s="20"/>
-      <c r="D52" s="20"/>
-      <c r="E52" s="21"/>
-    </row>
-    <row r="53" spans="1:5" ht="12">
-      <c r="A53" s="23"/>
-      <c r="B53" s="20"/>
-      <c r="C53" s="20"/>
-      <c r="D53" s="20"/>
-      <c r="E53" s="21"/>
-    </row>
-    <row r="54" spans="1:5" ht="12">
-      <c r="A54" s="23"/>
-      <c r="B54" s="20"/>
-      <c r="C54" s="20"/>
-      <c r="D54" s="20"/>
-      <c r="E54" s="21"/>
-    </row>
-    <row r="55" spans="1:5" ht="12">
-      <c r="A55" s="23"/>
-      <c r="B55" s="20"/>
-      <c r="C55" s="20"/>
-      <c r="D55" s="20"/>
-      <c r="E55" s="21"/>
-    </row>
-    <row r="56" spans="1:5" ht="12">
-      <c r="A56" s="23"/>
-      <c r="B56" s="20"/>
-      <c r="C56" s="20"/>
-      <c r="D56" s="20"/>
-      <c r="E56" s="21"/>
-    </row>
-    <row r="57" spans="1:5" ht="12">
-      <c r="A57" s="23"/>
-      <c r="B57" s="20"/>
-      <c r="C57" s="20"/>
-      <c r="D57" s="20"/>
-      <c r="E57" s="21"/>
-    </row>
-    <row r="58" spans="1:5" ht="12">
-      <c r="A58" s="23"/>
-      <c r="B58" s="20"/>
-      <c r="C58" s="20"/>
-      <c r="D58" s="20"/>
-      <c r="E58" s="21"/>
-    </row>
-    <row r="59" spans="1:5" ht="12">
-      <c r="A59" s="23"/>
-      <c r="B59" s="20"/>
-      <c r="C59" s="20"/>
-      <c r="D59" s="20"/>
-      <c r="E59" s="21"/>
-    </row>
-    <row r="60" spans="1:5" ht="12">
-      <c r="A60" s="23"/>
-      <c r="B60" s="20"/>
-      <c r="C60" s="20"/>
-      <c r="D60" s="20"/>
-      <c r="E60" s="21"/>
-    </row>
-    <row r="61" spans="1:5" ht="30" customHeight="1">
-      <c r="A61" s="19" t="s">
-        <v>48</v>
-      </c>
-      <c r="B61" s="20"/>
-      <c r="C61" s="20"/>
-      <c r="D61" s="20"/>
-      <c r="E61" s="21"/>
-    </row>
-    <row r="62" spans="1:5" ht="12" customHeight="1">
-      <c r="A62" s="36" t="s">
+      <c r="B51" s="22"/>
+      <c r="C51" s="22"/>
+      <c r="D51" s="22"/>
+      <c r="E51" s="23"/>
+    </row>
+    <row r="52" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A52" s="26"/>
+      <c r="B52" s="22"/>
+      <c r="C52" s="22"/>
+      <c r="D52" s="22"/>
+      <c r="E52" s="23"/>
+    </row>
+    <row r="53" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A53" s="25"/>
+      <c r="B53" s="22"/>
+      <c r="C53" s="22"/>
+      <c r="D53" s="22"/>
+      <c r="E53" s="23"/>
+    </row>
+    <row r="54" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A54" s="25"/>
+      <c r="B54" s="22"/>
+      <c r="C54" s="22"/>
+      <c r="D54" s="22"/>
+      <c r="E54" s="23"/>
+    </row>
+    <row r="55" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A55" s="25"/>
+      <c r="B55" s="22"/>
+      <c r="C55" s="22"/>
+      <c r="D55" s="22"/>
+      <c r="E55" s="23"/>
+    </row>
+    <row r="56" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A56" s="25"/>
+      <c r="B56" s="22"/>
+      <c r="C56" s="22"/>
+      <c r="D56" s="22"/>
+      <c r="E56" s="23"/>
+    </row>
+    <row r="57" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A57" s="25"/>
+      <c r="B57" s="22"/>
+      <c r="C57" s="22"/>
+      <c r="D57" s="22"/>
+      <c r="E57" s="23"/>
+    </row>
+    <row r="58" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A58" s="25"/>
+      <c r="B58" s="22"/>
+      <c r="C58" s="22"/>
+      <c r="D58" s="22"/>
+      <c r="E58" s="23"/>
+    </row>
+    <row r="59" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A59" s="25"/>
+      <c r="B59" s="22"/>
+      <c r="C59" s="22"/>
+      <c r="D59" s="22"/>
+      <c r="E59" s="23"/>
+    </row>
+    <row r="60" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A60" s="25"/>
+      <c r="B60" s="22"/>
+      <c r="C60" s="22"/>
+      <c r="D60" s="22"/>
+      <c r="E60" s="23"/>
+    </row>
+    <row r="61" spans="1:5" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="B61" s="22"/>
+      <c r="C61" s="22"/>
+      <c r="D61" s="22"/>
+      <c r="E61" s="23"/>
+    </row>
+    <row r="62" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="38" t="s">
         <v>41</v>
       </c>
-      <c r="B62" s="37"/>
-      <c r="C62" s="38"/>
-      <c r="D62" s="39" t="s">
+      <c r="B62" s="39"/>
+      <c r="C62" s="40"/>
+      <c r="D62" s="41" t="s">
         <v>42</v>
       </c>
-      <c r="E62" s="40"/>
-    </row>
-    <row r="63" spans="1:5" ht="12">
-      <c r="A63" s="30" t="s">
+      <c r="E62" s="42"/>
+    </row>
+    <row r="63" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A63" s="32" t="s">
+        <v>58</v>
+      </c>
+      <c r="B63" s="33"/>
+      <c r="C63" s="34"/>
+      <c r="D63" s="33" t="s">
+        <v>43</v>
+      </c>
+      <c r="E63" s="43"/>
+    </row>
+    <row r="64" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A64" s="32"/>
+      <c r="B64" s="33"/>
+      <c r="C64" s="34"/>
+      <c r="D64" s="33"/>
+      <c r="E64" s="43"/>
+    </row>
+    <row r="65" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A65" s="32"/>
+      <c r="B65" s="33"/>
+      <c r="C65" s="34"/>
+      <c r="D65" s="33"/>
+      <c r="E65" s="43"/>
+    </row>
+    <row r="66" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A66" s="32"/>
+      <c r="B66" s="33"/>
+      <c r="C66" s="34"/>
+      <c r="D66" s="33"/>
+      <c r="E66" s="43"/>
+    </row>
+    <row r="67" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A67" s="35"/>
+      <c r="B67" s="36"/>
+      <c r="C67" s="37"/>
+      <c r="D67" s="33"/>
+      <c r="E67" s="43"/>
+    </row>
+    <row r="68" spans="1:5" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A68" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="B63" s="31"/>
-      <c r="C63" s="32"/>
-      <c r="D63" s="31" t="s">
-        <v>43</v>
-      </c>
-      <c r="E63" s="41"/>
-    </row>
-    <row r="64" spans="1:5" ht="12">
-      <c r="A64" s="30"/>
-      <c r="B64" s="31"/>
-      <c r="C64" s="32"/>
-      <c r="D64" s="31"/>
-      <c r="E64" s="41"/>
-    </row>
-    <row r="65" spans="1:5" ht="12">
-      <c r="A65" s="30"/>
-      <c r="B65" s="31"/>
-      <c r="C65" s="32"/>
-      <c r="D65" s="31"/>
-      <c r="E65" s="41"/>
-    </row>
-    <row r="66" spans="1:5" ht="12">
-      <c r="A66" s="30"/>
-      <c r="B66" s="31"/>
-      <c r="C66" s="32"/>
-      <c r="D66" s="31"/>
-      <c r="E66" s="41"/>
-    </row>
-    <row r="67" spans="1:5" ht="12">
-      <c r="A67" s="33"/>
-      <c r="B67" s="34"/>
-      <c r="C67" s="35"/>
-      <c r="D67" s="31"/>
-      <c r="E67" s="41"/>
-    </row>
-    <row r="68" spans="1:5" ht="13" customHeight="1">
-      <c r="A68" s="19" t="s">
+      <c r="B68" s="22"/>
+      <c r="C68" s="22"/>
+      <c r="D68" s="22"/>
+      <c r="E68" s="23"/>
+    </row>
+    <row r="69" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A69" s="24"/>
+      <c r="B69" s="22"/>
+      <c r="C69" s="22"/>
+      <c r="D69" s="22"/>
+      <c r="E69" s="23"/>
+    </row>
+    <row r="70" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A70" s="25"/>
+      <c r="B70" s="22"/>
+      <c r="C70" s="22"/>
+      <c r="D70" s="22"/>
+      <c r="E70" s="23"/>
+    </row>
+    <row r="71" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A71" s="25"/>
+      <c r="B71" s="22"/>
+      <c r="C71" s="22"/>
+      <c r="D71" s="22"/>
+      <c r="E71" s="23"/>
+    </row>
+    <row r="72" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A72" s="25"/>
+      <c r="B72" s="22"/>
+      <c r="C72" s="22"/>
+      <c r="D72" s="22"/>
+      <c r="E72" s="23"/>
+    </row>
+    <row r="73" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A73" s="25"/>
+      <c r="B73" s="22"/>
+      <c r="C73" s="22"/>
+      <c r="D73" s="22"/>
+      <c r="E73" s="23"/>
+    </row>
+    <row r="74" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A74" s="25"/>
+      <c r="B74" s="22"/>
+      <c r="C74" s="22"/>
+      <c r="D74" s="22"/>
+      <c r="E74" s="23"/>
+    </row>
+    <row r="75" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A75" s="25"/>
+      <c r="B75" s="22"/>
+      <c r="C75" s="22"/>
+      <c r="D75" s="22"/>
+      <c r="E75" s="23"/>
+    </row>
+    <row r="76" spans="1:5" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A76" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="B68" s="20"/>
-      <c r="C68" s="20"/>
-      <c r="D68" s="20"/>
-      <c r="E68" s="21"/>
-    </row>
-    <row r="69" spans="1:5" ht="12">
-      <c r="A69" s="22"/>
-      <c r="B69" s="20"/>
-      <c r="C69" s="20"/>
-      <c r="D69" s="20"/>
-      <c r="E69" s="21"/>
-    </row>
-    <row r="70" spans="1:5" ht="12">
-      <c r="A70" s="23"/>
-      <c r="B70" s="20"/>
-      <c r="C70" s="20"/>
-      <c r="D70" s="20"/>
-      <c r="E70" s="21"/>
-    </row>
-    <row r="71" spans="1:5" ht="12">
-      <c r="A71" s="23"/>
-      <c r="B71" s="20"/>
-      <c r="C71" s="20"/>
-      <c r="D71" s="20"/>
-      <c r="E71" s="21"/>
-    </row>
-    <row r="72" spans="1:5" ht="12">
-      <c r="A72" s="23"/>
-      <c r="B72" s="20"/>
-      <c r="C72" s="20"/>
-      <c r="D72" s="20"/>
-      <c r="E72" s="21"/>
-    </row>
-    <row r="73" spans="1:5" ht="12">
-      <c r="A73" s="23"/>
-      <c r="B73" s="20"/>
-      <c r="C73" s="20"/>
-      <c r="D73" s="20"/>
-      <c r="E73" s="21"/>
-    </row>
-    <row r="74" spans="1:5" ht="12">
-      <c r="A74" s="23"/>
-      <c r="B74" s="20"/>
-      <c r="C74" s="20"/>
-      <c r="D74" s="20"/>
-      <c r="E74" s="21"/>
-    </row>
-    <row r="75" spans="1:5" ht="12">
-      <c r="A75" s="23"/>
-      <c r="B75" s="20"/>
-      <c r="C75" s="20"/>
-      <c r="D75" s="20"/>
-      <c r="E75" s="21"/>
-    </row>
-    <row r="76" spans="1:5" ht="13" customHeight="1">
-      <c r="A76" s="19" t="s">
+      <c r="B76" s="22"/>
+      <c r="C76" s="22"/>
+      <c r="D76" s="22"/>
+      <c r="E76" s="23"/>
+    </row>
+    <row r="77" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A77" s="26"/>
+      <c r="B77" s="22"/>
+      <c r="C77" s="22"/>
+      <c r="D77" s="22"/>
+      <c r="E77" s="23"/>
+    </row>
+    <row r="78" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A78" s="25"/>
+      <c r="B78" s="22"/>
+      <c r="C78" s="22"/>
+      <c r="D78" s="22"/>
+      <c r="E78" s="23"/>
+    </row>
+    <row r="79" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A79" s="25"/>
+      <c r="B79" s="22"/>
+      <c r="C79" s="22"/>
+      <c r="D79" s="22"/>
+      <c r="E79" s="23"/>
+    </row>
+    <row r="80" spans="1:5" s="18" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A80" s="25"/>
+      <c r="B80" s="22"/>
+      <c r="C80" s="22"/>
+      <c r="D80" s="22"/>
+      <c r="E80" s="23"/>
+    </row>
+    <row r="81" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A81" s="25"/>
+      <c r="B81" s="22"/>
+      <c r="C81" s="22"/>
+      <c r="D81" s="22"/>
+      <c r="E81" s="23"/>
+    </row>
+    <row r="82" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A82" s="25"/>
+      <c r="B82" s="22"/>
+      <c r="C82" s="22"/>
+      <c r="D82" s="22"/>
+      <c r="E82" s="23"/>
+    </row>
+    <row r="83" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A83" s="25"/>
+      <c r="B83" s="22"/>
+      <c r="C83" s="22"/>
+      <c r="D83" s="22"/>
+      <c r="E83" s="23"/>
+    </row>
+    <row r="84" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A84" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="B76" s="20"/>
-      <c r="C76" s="20"/>
-      <c r="D76" s="20"/>
-      <c r="E76" s="21"/>
-    </row>
-    <row r="77" spans="1:5" ht="12">
-      <c r="A77" s="24"/>
-      <c r="B77" s="20"/>
-      <c r="C77" s="20"/>
-      <c r="D77" s="20"/>
-      <c r="E77" s="21"/>
-    </row>
-    <row r="78" spans="1:5" ht="12">
-      <c r="A78" s="23"/>
-      <c r="B78" s="20"/>
-      <c r="C78" s="20"/>
-      <c r="D78" s="20"/>
-      <c r="E78" s="21"/>
-    </row>
-    <row r="79" spans="1:5" ht="12">
-      <c r="A79" s="23"/>
-      <c r="B79" s="20"/>
-      <c r="C79" s="20"/>
-      <c r="D79" s="20"/>
-      <c r="E79" s="21"/>
-    </row>
-    <row r="80" spans="1:5" s="18" customFormat="1" ht="12">
-      <c r="A80" s="23"/>
-      <c r="B80" s="20"/>
-      <c r="C80" s="20"/>
-      <c r="D80" s="20"/>
-      <c r="E80" s="21"/>
-    </row>
-    <row r="81" spans="1:5" ht="12">
-      <c r="A81" s="23"/>
-      <c r="B81" s="20"/>
-      <c r="C81" s="20"/>
-      <c r="D81" s="20"/>
-      <c r="E81" s="21"/>
-    </row>
-    <row r="82" spans="1:5" ht="12">
-      <c r="A82" s="23"/>
-      <c r="B82" s="20"/>
-      <c r="C82" s="20"/>
-      <c r="D82" s="20"/>
-      <c r="E82" s="21"/>
-    </row>
-    <row r="83" spans="1:5" ht="12">
-      <c r="A83" s="23"/>
-      <c r="B83" s="20"/>
-      <c r="C83" s="20"/>
-      <c r="D83" s="20"/>
-      <c r="E83" s="21"/>
-    </row>
-    <row r="84" spans="1:5" ht="30" customHeight="1">
-      <c r="A84" s="25" t="s">
-        <v>47</v>
-      </c>
-      <c r="B84" s="20"/>
-      <c r="C84" s="20"/>
-      <c r="D84" s="20"/>
-      <c r="E84" s="21"/>
-    </row>
-    <row r="85" spans="1:5" ht="12">
-      <c r="A85" s="24"/>
-      <c r="B85" s="20"/>
-      <c r="C85" s="20"/>
-      <c r="D85" s="20"/>
-      <c r="E85" s="21"/>
-    </row>
-    <row r="86" spans="1:5" ht="12">
-      <c r="A86" s="23"/>
-      <c r="B86" s="20"/>
-      <c r="C86" s="20"/>
-      <c r="D86" s="20"/>
-      <c r="E86" s="21"/>
-    </row>
-    <row r="87" spans="1:5" ht="12">
-      <c r="A87" s="23"/>
-      <c r="B87" s="20"/>
-      <c r="C87" s="20"/>
-      <c r="D87" s="20"/>
-      <c r="E87" s="21"/>
-    </row>
-    <row r="88" spans="1:5" s="18" customFormat="1" ht="12">
-      <c r="A88" s="23"/>
-      <c r="B88" s="20"/>
-      <c r="C88" s="20"/>
-      <c r="D88" s="20"/>
-      <c r="E88" s="21"/>
-    </row>
-    <row r="89" spans="1:5" ht="12">
-      <c r="A89" s="23"/>
-      <c r="B89" s="20"/>
-      <c r="C89" s="20"/>
-      <c r="D89" s="20"/>
-      <c r="E89" s="21"/>
-    </row>
-    <row r="90" spans="1:5" ht="12">
-      <c r="A90" s="23"/>
-      <c r="B90" s="20"/>
-      <c r="C90" s="20"/>
-      <c r="D90" s="20"/>
-      <c r="E90" s="21"/>
-    </row>
-    <row r="91" spans="1:5" ht="12">
-      <c r="A91" s="23"/>
-      <c r="B91" s="20"/>
-      <c r="C91" s="20"/>
-      <c r="D91" s="20"/>
-      <c r="E91" s="21"/>
-    </row>
-    <row r="92" spans="1:5" ht="15" customHeight="1">
+      <c r="B84" s="22"/>
+      <c r="C84" s="22"/>
+      <c r="D84" s="22"/>
+      <c r="E84" s="23"/>
+    </row>
+    <row r="85" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A85" s="26"/>
+      <c r="B85" s="22"/>
+      <c r="C85" s="22"/>
+      <c r="D85" s="22"/>
+      <c r="E85" s="23"/>
+    </row>
+    <row r="86" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A86" s="25"/>
+      <c r="B86" s="22"/>
+      <c r="C86" s="22"/>
+      <c r="D86" s="22"/>
+      <c r="E86" s="23"/>
+    </row>
+    <row r="87" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A87" s="25"/>
+      <c r="B87" s="22"/>
+      <c r="C87" s="22"/>
+      <c r="D87" s="22"/>
+      <c r="E87" s="23"/>
+    </row>
+    <row r="88" spans="1:5" s="18" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A88" s="25"/>
+      <c r="B88" s="22"/>
+      <c r="C88" s="22"/>
+      <c r="D88" s="22"/>
+      <c r="E88" s="23"/>
+    </row>
+    <row r="89" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A89" s="25"/>
+      <c r="B89" s="22"/>
+      <c r="C89" s="22"/>
+      <c r="D89" s="22"/>
+      <c r="E89" s="23"/>
+    </row>
+    <row r="90" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A90" s="25"/>
+      <c r="B90" s="22"/>
+      <c r="C90" s="22"/>
+      <c r="D90" s="22"/>
+      <c r="E90" s="23"/>
+    </row>
+    <row r="91" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A91" s="25"/>
+      <c r="B91" s="22"/>
+      <c r="C91" s="22"/>
+      <c r="D91" s="22"/>
+      <c r="E91" s="23"/>
+    </row>
+    <row r="92" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="13" t="s">
         <v>28</v>
       </c>
@@ -2103,17 +2127,17 @@
       <c r="D92" s="3"/>
       <c r="E92" s="3"/>
     </row>
-    <row r="93" spans="1:5" ht="4.5" customHeight="1"/>
-    <row r="94" spans="1:5" ht="13">
-      <c r="A94" s="29" t="s">
+    <row r="93" spans="1:5" ht="4.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A94" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="B94" s="27"/>
-      <c r="C94" s="27"/>
-      <c r="D94" s="27"/>
-      <c r="E94" s="27"/>
-    </row>
-    <row r="95" spans="1:5" ht="13">
+      <c r="B94" s="29"/>
+      <c r="C94" s="29"/>
+      <c r="D94" s="29"/>
+      <c r="E94" s="29"/>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A95" s="2" t="s">
         <v>30</v>
       </c>
@@ -2121,7 +2145,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="96" spans="1:5" ht="13">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A96" s="2" t="s">
         <v>32</v>
       </c>
@@ -2129,7 +2153,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="97" spans="1:5" ht="13">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A97" s="2" t="s">
         <v>34</v>
       </c>
@@ -2137,7 +2161,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="98" spans="1:5" ht="39">
+    <row r="98" spans="1:5" ht="57" x14ac:dyDescent="0.2">
       <c r="A98" s="15" t="s">
         <v>36</v>
       </c>
@@ -2145,93 +2169,116 @@
         <v>37</v>
       </c>
     </row>
-    <row r="100" spans="1:5" s="18" customFormat="1" ht="13" customHeight="1">
-      <c r="A100" s="26" t="s">
-        <v>53</v>
-      </c>
-      <c r="B100" s="26"/>
-      <c r="C100" s="26"/>
-      <c r="D100" s="26"/>
-      <c r="E100" s="26"/>
-    </row>
-    <row r="101" spans="1:5" s="18" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="102" spans="1:5" ht="13" customHeight="1">
-      <c r="A102" s="26" t="s">
+    <row r="99" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="100" spans="1:5" s="18" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A100" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="B100" s="28"/>
+      <c r="C100" s="28"/>
+      <c r="D100" s="28"/>
+      <c r="E100" s="28"/>
+    </row>
+    <row r="101" spans="1:5" s="18" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="102" spans="1:5" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A102" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="B102" s="29"/>
+      <c r="C102" s="29"/>
+    </row>
+    <row r="103" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="104" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A104" s="28" t="s">
+        <v>55</v>
+      </c>
+      <c r="B104" s="29"/>
+      <c r="C104" s="29"/>
+      <c r="D104" s="29"/>
+      <c r="E104" s="29"/>
+    </row>
+    <row r="105" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="106" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A106" s="28" t="s">
+        <v>56</v>
+      </c>
+      <c r="B106" s="29"/>
+      <c r="C106" s="29"/>
+      <c r="D106" s="29"/>
+      <c r="E106" s="29"/>
+    </row>
+    <row r="107" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="108" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A108" s="28" t="s">
+        <v>54</v>
+      </c>
+      <c r="B108" s="29"/>
+      <c r="C108" s="29"/>
+      <c r="D108" s="29"/>
+      <c r="E108" s="29"/>
+    </row>
+    <row r="109" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="110" spans="1:5" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A110" s="28" t="s">
+        <v>57</v>
+      </c>
+      <c r="B110" s="29"/>
+      <c r="C110" s="29"/>
+      <c r="D110" s="29"/>
+      <c r="E110" s="29"/>
+    </row>
+    <row r="111" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="112" spans="1:5" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A112" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="B102" s="27"/>
-      <c r="C102" s="27"/>
-    </row>
-    <row r="104" spans="1:5" ht="30" customHeight="1">
-      <c r="A104" s="26" t="s">
-        <v>56</v>
-      </c>
-      <c r="B104" s="27"/>
-      <c r="C104" s="27"/>
-      <c r="D104" s="27"/>
-      <c r="E104" s="27"/>
-    </row>
-    <row r="106" spans="1:5" ht="30" customHeight="1">
-      <c r="A106" s="26" t="s">
-        <v>57</v>
-      </c>
-      <c r="B106" s="27"/>
-      <c r="C106" s="27"/>
-      <c r="D106" s="27"/>
-      <c r="E106" s="27"/>
-    </row>
-    <row r="108" spans="1:5" ht="30" customHeight="1">
-      <c r="A108" s="26" t="s">
-        <v>55</v>
-      </c>
-      <c r="B108" s="27"/>
-      <c r="C108" s="27"/>
-      <c r="D108" s="27"/>
-      <c r="E108" s="27"/>
-    </row>
-    <row r="110" spans="1:5" ht="40" customHeight="1">
-      <c r="A110" s="26" t="s">
-        <v>58</v>
-      </c>
-      <c r="B110" s="27"/>
-      <c r="C110" s="27"/>
-      <c r="D110" s="27"/>
-      <c r="E110" s="27"/>
-    </row>
-    <row r="112" spans="1:5" ht="40" customHeight="1">
-      <c r="A112" s="26" t="s">
-        <v>51</v>
-      </c>
-      <c r="B112" s="28"/>
-      <c r="C112" s="28"/>
-      <c r="D112" s="28"/>
-      <c r="E112" s="28"/>
-    </row>
-    <row r="113" spans="1:5" ht="14" customHeight="1">
+      <c r="B112" s="30"/>
+      <c r="C112" s="30"/>
+      <c r="D112" s="30"/>
+      <c r="E112" s="30"/>
+    </row>
+    <row r="113" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113" s="16"/>
       <c r="B113" s="17"/>
       <c r="C113" s="17"/>
       <c r="D113" s="17"/>
       <c r="E113" s="17"/>
     </row>
-    <row r="114" spans="1:5" ht="40" customHeight="1">
-      <c r="A114" s="26" t="s">
-        <v>52</v>
-      </c>
-      <c r="B114" s="26"/>
-      <c r="C114" s="26"/>
-      <c r="D114" s="26"/>
-      <c r="E114" s="26"/>
-    </row>
-    <row r="116" spans="1:5" ht="30.75" customHeight="1">
-      <c r="A116" s="26" t="s">
-        <v>54</v>
-      </c>
-      <c r="B116" s="27"/>
-      <c r="C116" s="27"/>
-      <c r="D116" s="27"/>
-      <c r="E116" s="27"/>
-    </row>
+    <row r="114" spans="1:5" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A114" s="28" t="s">
+        <v>51</v>
+      </c>
+      <c r="B114" s="28"/>
+      <c r="C114" s="28"/>
+      <c r="D114" s="28"/>
+      <c r="E114" s="28"/>
+    </row>
+    <row r="115" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="116" spans="1:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A116" s="28" t="s">
+        <v>53</v>
+      </c>
+      <c r="B116" s="29"/>
+      <c r="C116" s="29"/>
+      <c r="D116" s="29"/>
+      <c r="E116" s="29"/>
+    </row>
+    <row r="117" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="118" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="119" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="120" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="121" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="122" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="123" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="124" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="125" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="126" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="127" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="128" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="129" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="130" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="131" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="132" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="62">
     <mergeCell ref="A1:E1"/>
@@ -2299,10 +2346,10 @@
   </mergeCells>
   <phoneticPr fontId="26" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+      <mx:PLV Mode="1" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
 </worksheet>
@@ -2314,7 +2361,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <phoneticPr fontId="26" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2333,7 +2380,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <phoneticPr fontId="26" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
updated recommendation and app forms
</commit_message>
<xml_diff>
--- a/app/assets/files/NAPI 2013 Application Form.xlsx
+++ b/app/assets/files/NAPI 2013 Application Form.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23416"/>
   <workbookPr checkCompatibility="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-735" yWindow="-21045" windowWidth="20730" windowHeight="11760" tabRatio="500"/>
+    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="13940" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Application" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
@@ -218,6 +218,9 @@
     <t>1 year</t>
   </si>
   <si>
+    <t>Example:  Experience with vacuum systems</t>
+  </si>
+  <si>
     <t>4. Why should you be accepted into this program? (100 words)</t>
   </si>
   <si>
@@ -328,31 +331,17 @@
     </r>
   </si>
   <si>
-    <t>5. Send the PDF files to internship.naist@gmail.com on or before July 19, 2013 23:59 GMT+8 with NAPI2013 Application as the subject line of your email.</t>
-  </si>
-  <si>
-    <t>7. Deadline for the recommendation form is on or before July 19, 2013 23:59 GMT+8. Please contact your professors/advisers beforehand about your application. Kindly ask them to send the document directly to internship.naist@gmail.com in PDF format.</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Example:  Experience with vacuum systems </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t>(Kindly delete this when filling this part)</t>
-    </r>
+    <t>5. Send the PDF files to internship.naist@gmail.com on or before July 19, 2013 11:59 PM (Philippine standard time) with NAPI2013 Application as the subject line of your email.</t>
+  </si>
+  <si>
+    <t>7. Deadline for the recommendation form is on or before July 19, 2013 11:59 PM (Philippine standard time). Please contact your professors/advisers beforehand about your application. Kindly ask them to send the document directly to internship.naist@gmail.com in PDF format.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="32" x14ac:knownFonts="1">
+  <fonts count="31" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -513,12 +502,6 @@
       <u/>
       <sz val="10"/>
       <color theme="11"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
   </fonts>
@@ -926,134 +909,134 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1062,11 +1045,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -1392,48 +1370,46 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F132"/>
+  <dimension ref="A1:E116"/>
   <sheetViews>
-    <sheetView tabSelected="1" showWhiteSpace="0" view="pageLayout" workbookViewId="0">
-      <selection activeCell="D66" sqref="D66:E66"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22:E24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.25" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14.25" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="3" width="23" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" customWidth="1"/>
-    <col min="6" max="6" width="2.140625" hidden="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" hidden="1"/>
+    <col min="4" max="4" width="12.6640625" customWidth="1"/>
+    <col min="5" max="5" width="9.1640625" customWidth="1"/>
+    <col min="6" max="6" width="2.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="49" t="s">
+    <row r="1" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A1" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-    </row>
-    <row r="2" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="45" t="s">
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+    </row>
+    <row r="3" spans="1:5" ht="13">
+      <c r="A3" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="46"/>
-      <c r="C3" s="46"/>
-      <c r="D3" s="46"/>
-      <c r="E3" s="46"/>
-    </row>
-    <row r="4" spans="1:5" ht="6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="44"/>
+      <c r="C3" s="44"/>
+      <c r="D3" s="44"/>
+      <c r="E3" s="44"/>
+    </row>
+    <row r="4" spans="1:5" ht="6" customHeight="1">
       <c r="A4" s="10"/>
       <c r="B4" s="10"/>
       <c r="C4" s="10"/>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" ht="13">
       <c r="A5" s="4" t="s">
         <v>2</v>
       </c>
@@ -1443,19 +1419,19 @@
       <c r="C5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="61" t="s">
+      <c r="D5" s="59" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="57"/>
-    </row>
-    <row r="6" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E5" s="60"/>
+    </row>
+    <row r="6" spans="1:5" ht="30" customHeight="1">
       <c r="A6" s="11"/>
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
-      <c r="D6" s="25"/>
-      <c r="E6" s="57"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D6" s="23"/>
+      <c r="E6" s="60"/>
+    </row>
+    <row r="7" spans="1:5" ht="13">
       <c r="A7" s="4" t="s">
         <v>6</v>
       </c>
@@ -1465,130 +1441,130 @@
       <c r="C7" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="25"/>
-      <c r="E7" s="57"/>
-    </row>
-    <row r="8" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D7" s="23"/>
+      <c r="E7" s="60"/>
+    </row>
+    <row r="8" spans="1:5" ht="30" customHeight="1">
       <c r="A8" s="11"/>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
-      <c r="D8" s="25"/>
-      <c r="E8" s="57"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="62" t="s">
+      <c r="D8" s="23"/>
+      <c r="E8" s="60"/>
+    </row>
+    <row r="9" spans="1:5" ht="13">
+      <c r="A9" s="58" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="23"/>
+      <c r="B9" s="21"/>
       <c r="C9" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="25"/>
-      <c r="E9" s="57"/>
-    </row>
-    <row r="10" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="60"/>
-      <c r="B10" s="23"/>
+      <c r="D9" s="23"/>
+      <c r="E9" s="60"/>
+    </row>
+    <row r="10" spans="1:5" ht="30" customHeight="1">
+      <c r="A10" s="57"/>
+      <c r="B10" s="21"/>
       <c r="C10" s="11"/>
-      <c r="D10" s="25"/>
-      <c r="E10" s="57"/>
-    </row>
-    <row r="11" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D10" s="23"/>
+      <c r="E10" s="60"/>
+    </row>
+    <row r="11" spans="1:5" ht="25" customHeight="1">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="45" t="s">
+    <row r="12" spans="1:5" ht="13">
+      <c r="A12" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="46"/>
-      <c r="C12" s="46"/>
-      <c r="D12" s="46"/>
-      <c r="E12" s="46"/>
-    </row>
-    <row r="13" spans="1:5" ht="6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="44"/>
+      <c r="C12" s="44"/>
+      <c r="D12" s="44"/>
+      <c r="E12" s="44"/>
+    </row>
+    <row r="13" spans="1:5" ht="6" customHeight="1">
       <c r="A13" s="10"/>
       <c r="B13" s="10"/>
       <c r="C13" s="10"/>
       <c r="D13" s="10"/>
       <c r="E13" s="10"/>
     </row>
-    <row r="14" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="56" t="s">
+    <row r="14" spans="1:5" ht="30" customHeight="1">
+      <c r="A14" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="23"/>
+      <c r="B14" s="21"/>
       <c r="C14" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="59" t="s">
+      <c r="D14" s="56" t="s">
         <v>14</v>
       </c>
-      <c r="E14" s="57"/>
-    </row>
-    <row r="15" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="60"/>
-      <c r="B15" s="23"/>
+      <c r="E14" s="60"/>
+    </row>
+    <row r="15" spans="1:5" ht="30" customHeight="1">
+      <c r="A15" s="57"/>
+      <c r="B15" s="21"/>
       <c r="C15" s="11"/>
-      <c r="D15" s="51"/>
-      <c r="E15" s="57"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="56" t="s">
+      <c r="D15" s="49"/>
+      <c r="E15" s="60"/>
+    </row>
+    <row r="16" spans="1:5" ht="13">
+      <c r="A16" s="54" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="48"/>
-      <c r="C16" s="23"/>
-      <c r="D16" s="50" t="s">
+      <c r="B16" s="46"/>
+      <c r="C16" s="21"/>
+      <c r="D16" s="48" t="s">
         <v>16</v>
       </c>
-      <c r="E16" s="57"/>
-    </row>
-    <row r="17" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="51"/>
-      <c r="B17" s="48"/>
-      <c r="C17" s="23"/>
-      <c r="D17" s="51"/>
-      <c r="E17" s="57"/>
-    </row>
-    <row r="18" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="58" t="s">
+      <c r="E16" s="60"/>
+    </row>
+    <row r="17" spans="1:5" ht="30" customHeight="1">
+      <c r="A17" s="49"/>
+      <c r="B17" s="46"/>
+      <c r="C17" s="21"/>
+      <c r="D17" s="49"/>
+      <c r="E17" s="60"/>
+    </row>
+    <row r="18" spans="1:5" ht="30" customHeight="1">
+      <c r="A18" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="B18" s="22"/>
-      <c r="C18" s="22"/>
-      <c r="D18" s="22"/>
-      <c r="E18" s="57"/>
-    </row>
-    <row r="19" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="51"/>
-      <c r="B19" s="48"/>
-      <c r="C19" s="48"/>
-      <c r="D19" s="48"/>
-      <c r="E19" s="22"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" s="52" t="s">
+      <c r="B18" s="20"/>
+      <c r="C18" s="20"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="60"/>
+    </row>
+    <row r="19" spans="1:5" ht="30" customHeight="1">
+      <c r="A19" s="49"/>
+      <c r="B19" s="46"/>
+      <c r="C19" s="46"/>
+      <c r="D19" s="46"/>
+      <c r="E19" s="20"/>
+    </row>
+    <row r="20" spans="1:5" ht="13">
+      <c r="A20" s="50" t="s">
         <v>17</v>
       </c>
-      <c r="B20" s="22"/>
-      <c r="C20" s="22"/>
-      <c r="D20" s="22"/>
-      <c r="E20" s="23"/>
-    </row>
-    <row r="21" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="53" t="s">
-        <v>48</v>
-      </c>
-      <c r="B21" s="54"/>
-      <c r="C21" s="54"/>
-      <c r="D21" s="54"/>
-      <c r="E21" s="55"/>
-    </row>
-    <row r="22" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B20" s="20"/>
+      <c r="C20" s="20"/>
+      <c r="D20" s="20"/>
+      <c r="E20" s="21"/>
+    </row>
+    <row r="21" spans="1:5" ht="30" customHeight="1">
+      <c r="A21" s="51" t="s">
+        <v>49</v>
+      </c>
+      <c r="B21" s="52"/>
+      <c r="C21" s="52"/>
+      <c r="D21" s="52"/>
+      <c r="E21" s="53"/>
+    </row>
+    <row r="22" spans="1:5" ht="30" customHeight="1">
       <c r="A22" s="8" t="s">
         <v>18</v>
       </c>
@@ -1597,9 +1573,9 @@
       </c>
       <c r="C22" s="7"/>
       <c r="D22" s="7"/>
-      <c r="E22" s="19"/>
-    </row>
-    <row r="23" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E22" s="61"/>
+    </row>
+    <row r="23" spans="1:5" ht="30" customHeight="1">
       <c r="A23" s="8" t="s">
         <v>20</v>
       </c>
@@ -1608,517 +1584,517 @@
       </c>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
-      <c r="E23" s="19"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E23" s="61"/>
+    </row>
+    <row r="24" spans="1:5" ht="13">
       <c r="A24" s="12"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
-      <c r="E24" s="20"/>
-    </row>
-    <row r="25" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E24" s="62"/>
+    </row>
+    <row r="25" spans="1:5" ht="25" customHeight="1">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26" s="45" t="s">
+    <row r="26" spans="1:5" ht="13">
+      <c r="A26" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="B26" s="46"/>
-      <c r="C26" s="46"/>
-      <c r="D26" s="46"/>
-      <c r="E26" s="46"/>
-    </row>
-    <row r="27" spans="1:5" ht="4.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B26" s="44"/>
+      <c r="C26" s="44"/>
+      <c r="D26" s="44"/>
+      <c r="E26" s="44"/>
+    </row>
+    <row r="27" spans="1:5" ht="4.5" customHeight="1">
       <c r="A27" s="10"/>
       <c r="B27" s="10"/>
       <c r="C27" s="10"/>
       <c r="D27" s="10"/>
       <c r="E27" s="10"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28" s="50" t="s">
+    <row r="28" spans="1:5" ht="13">
+      <c r="A28" s="48" t="s">
         <v>22</v>
       </c>
-      <c r="B28" s="22"/>
-      <c r="C28" s="22"/>
-      <c r="D28" s="22"/>
-      <c r="E28" s="23"/>
-    </row>
-    <row r="29" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="26"/>
-      <c r="B29" s="22"/>
-      <c r="C29" s="22"/>
-      <c r="D29" s="22"/>
-      <c r="E29" s="23"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A30" s="50" t="s">
+      <c r="B28" s="20"/>
+      <c r="C28" s="20"/>
+      <c r="D28" s="20"/>
+      <c r="E28" s="21"/>
+    </row>
+    <row r="29" spans="1:5" ht="22.5" customHeight="1">
+      <c r="A29" s="24"/>
+      <c r="B29" s="20"/>
+      <c r="C29" s="20"/>
+      <c r="D29" s="20"/>
+      <c r="E29" s="21"/>
+    </row>
+    <row r="30" spans="1:5" ht="13">
+      <c r="A30" s="48" t="s">
         <v>23</v>
       </c>
-      <c r="B30" s="22"/>
-      <c r="C30" s="22"/>
-      <c r="D30" s="22"/>
-      <c r="E30" s="23"/>
-    </row>
-    <row r="31" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="26"/>
-      <c r="B31" s="22"/>
-      <c r="C31" s="22"/>
-      <c r="D31" s="22"/>
-      <c r="E31" s="23"/>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A32" s="50" t="s">
+      <c r="B30" s="20"/>
+      <c r="C30" s="20"/>
+      <c r="D30" s="20"/>
+      <c r="E30" s="21"/>
+    </row>
+    <row r="31" spans="1:5" ht="22.5" customHeight="1">
+      <c r="A31" s="24"/>
+      <c r="B31" s="20"/>
+      <c r="C31" s="20"/>
+      <c r="D31" s="20"/>
+      <c r="E31" s="21"/>
+    </row>
+    <row r="32" spans="1:5" ht="13">
+      <c r="A32" s="48" t="s">
         <v>24</v>
       </c>
-      <c r="B32" s="22"/>
-      <c r="C32" s="22"/>
-      <c r="D32" s="22"/>
-      <c r="E32" s="23"/>
-    </row>
-    <row r="33" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="26"/>
-      <c r="B33" s="22"/>
-      <c r="C33" s="22"/>
-      <c r="D33" s="22"/>
-      <c r="E33" s="23"/>
-    </row>
-    <row r="34" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B32" s="20"/>
+      <c r="C32" s="20"/>
+      <c r="D32" s="20"/>
+      <c r="E32" s="21"/>
+    </row>
+    <row r="33" spans="1:5" ht="22.5" customHeight="1">
+      <c r="A33" s="24"/>
+      <c r="B33" s="20"/>
+      <c r="C33" s="20"/>
+      <c r="D33" s="20"/>
+      <c r="E33" s="21"/>
+    </row>
+    <row r="34" spans="1:5" ht="15" customHeight="1">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
       <c r="E34" s="3"/>
     </row>
-    <row r="35" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A35" s="44" t="s">
+    <row r="35" spans="1:5" ht="12">
+      <c r="A35" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="B35" s="29"/>
-      <c r="C35" s="29"/>
-      <c r="D35" s="29"/>
-      <c r="E35" s="29"/>
-    </row>
-    <row r="36" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B35" s="27"/>
+      <c r="C35" s="27"/>
+      <c r="D35" s="27"/>
+      <c r="E35" s="27"/>
+    </row>
+    <row r="36" spans="1:5" ht="22.5" customHeight="1">
       <c r="A36" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B36" s="45"/>
-      <c r="C36" s="46"/>
-    </row>
-    <row r="37" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B36" s="43"/>
+      <c r="C36" s="44"/>
+    </row>
+    <row r="37" spans="1:5" ht="22.5" customHeight="1">
       <c r="A37" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B37" s="47"/>
-      <c r="C37" s="48"/>
-    </row>
-    <row r="38" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="49" t="s">
+      <c r="B37" s="45"/>
+      <c r="C37" s="46"/>
+    </row>
+    <row r="38" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A38" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B38" s="29"/>
-      <c r="C38" s="29"/>
-      <c r="D38" s="29"/>
-      <c r="E38" s="29"/>
-    </row>
-    <row r="39" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B38" s="27"/>
+      <c r="C38" s="27"/>
+      <c r="D38" s="27"/>
+      <c r="E38" s="27"/>
+    </row>
+    <row r="39" spans="1:5" ht="12">
       <c r="A39" s="9"/>
       <c r="B39" s="9"/>
       <c r="C39" s="9"/>
       <c r="D39" s="9"/>
       <c r="E39" s="9"/>
     </row>
-    <row r="40" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="27" t="s">
+    <row r="40" spans="1:5" ht="30" customHeight="1">
+      <c r="A40" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="B40" s="22"/>
-      <c r="C40" s="22"/>
-      <c r="D40" s="22"/>
-      <c r="E40" s="23"/>
-    </row>
-    <row r="41" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A41" s="26"/>
-      <c r="B41" s="22"/>
-      <c r="C41" s="22"/>
-      <c r="D41" s="22"/>
-      <c r="E41" s="23"/>
-    </row>
-    <row r="42" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A42" s="25"/>
-      <c r="B42" s="22"/>
-      <c r="C42" s="22"/>
-      <c r="D42" s="22"/>
-      <c r="E42" s="23"/>
-    </row>
-    <row r="43" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A43" s="25"/>
-      <c r="B43" s="22"/>
-      <c r="C43" s="22"/>
-      <c r="D43" s="22"/>
-      <c r="E43" s="23"/>
-    </row>
-    <row r="44" spans="1:5" s="18" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A44" s="25"/>
-      <c r="B44" s="22"/>
-      <c r="C44" s="22"/>
-      <c r="D44" s="22"/>
-      <c r="E44" s="23"/>
-    </row>
-    <row r="45" spans="1:5" s="18" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A45" s="25"/>
-      <c r="B45" s="22"/>
-      <c r="C45" s="22"/>
-      <c r="D45" s="22"/>
-      <c r="E45" s="23"/>
-    </row>
-    <row r="46" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A46" s="25"/>
-      <c r="B46" s="22"/>
-      <c r="C46" s="22"/>
-      <c r="D46" s="22"/>
-      <c r="E46" s="23"/>
-    </row>
-    <row r="47" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A47" s="25"/>
-      <c r="B47" s="22"/>
-      <c r="C47" s="22"/>
-      <c r="D47" s="22"/>
-      <c r="E47" s="23"/>
-    </row>
-    <row r="48" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A48" s="25"/>
-      <c r="B48" s="22"/>
-      <c r="C48" s="22"/>
-      <c r="D48" s="22"/>
-      <c r="E48" s="23"/>
-    </row>
-    <row r="49" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A49" s="25"/>
-      <c r="B49" s="22"/>
-      <c r="C49" s="22"/>
-      <c r="D49" s="22"/>
-      <c r="E49" s="23"/>
-    </row>
-    <row r="50" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A50" s="25"/>
-      <c r="B50" s="22"/>
-      <c r="C50" s="22"/>
-      <c r="D50" s="22"/>
-      <c r="E50" s="23"/>
-    </row>
-    <row r="51" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="21" t="s">
+      <c r="B40" s="20"/>
+      <c r="C40" s="20"/>
+      <c r="D40" s="20"/>
+      <c r="E40" s="21"/>
+    </row>
+    <row r="41" spans="1:5" ht="12">
+      <c r="A41" s="24"/>
+      <c r="B41" s="20"/>
+      <c r="C41" s="20"/>
+      <c r="D41" s="20"/>
+      <c r="E41" s="21"/>
+    </row>
+    <row r="42" spans="1:5" ht="12">
+      <c r="A42" s="23"/>
+      <c r="B42" s="20"/>
+      <c r="C42" s="20"/>
+      <c r="D42" s="20"/>
+      <c r="E42" s="21"/>
+    </row>
+    <row r="43" spans="1:5" ht="12">
+      <c r="A43" s="23"/>
+      <c r="B43" s="20"/>
+      <c r="C43" s="20"/>
+      <c r="D43" s="20"/>
+      <c r="E43" s="21"/>
+    </row>
+    <row r="44" spans="1:5" s="18" customFormat="1" ht="12">
+      <c r="A44" s="23"/>
+      <c r="B44" s="20"/>
+      <c r="C44" s="20"/>
+      <c r="D44" s="20"/>
+      <c r="E44" s="21"/>
+    </row>
+    <row r="45" spans="1:5" s="18" customFormat="1" ht="12">
+      <c r="A45" s="23"/>
+      <c r="B45" s="20"/>
+      <c r="C45" s="20"/>
+      <c r="D45" s="20"/>
+      <c r="E45" s="21"/>
+    </row>
+    <row r="46" spans="1:5" ht="12">
+      <c r="A46" s="23"/>
+      <c r="B46" s="20"/>
+      <c r="C46" s="20"/>
+      <c r="D46" s="20"/>
+      <c r="E46" s="21"/>
+    </row>
+    <row r="47" spans="1:5" ht="12">
+      <c r="A47" s="23"/>
+      <c r="B47" s="20"/>
+      <c r="C47" s="20"/>
+      <c r="D47" s="20"/>
+      <c r="E47" s="21"/>
+    </row>
+    <row r="48" spans="1:5" ht="12">
+      <c r="A48" s="23"/>
+      <c r="B48" s="20"/>
+      <c r="C48" s="20"/>
+      <c r="D48" s="20"/>
+      <c r="E48" s="21"/>
+    </row>
+    <row r="49" spans="1:5" ht="12">
+      <c r="A49" s="23"/>
+      <c r="B49" s="20"/>
+      <c r="C49" s="20"/>
+      <c r="D49" s="20"/>
+      <c r="E49" s="21"/>
+    </row>
+    <row r="50" spans="1:5" ht="12">
+      <c r="A50" s="23"/>
+      <c r="B50" s="20"/>
+      <c r="C50" s="20"/>
+      <c r="D50" s="20"/>
+      <c r="E50" s="21"/>
+    </row>
+    <row r="51" spans="1:5" ht="30" customHeight="1">
+      <c r="A51" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="B51" s="22"/>
-      <c r="C51" s="22"/>
-      <c r="D51" s="22"/>
-      <c r="E51" s="23"/>
-    </row>
-    <row r="52" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A52" s="26"/>
-      <c r="B52" s="22"/>
-      <c r="C52" s="22"/>
-      <c r="D52" s="22"/>
-      <c r="E52" s="23"/>
-    </row>
-    <row r="53" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A53" s="25"/>
-      <c r="B53" s="22"/>
-      <c r="C53" s="22"/>
-      <c r="D53" s="22"/>
-      <c r="E53" s="23"/>
-    </row>
-    <row r="54" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A54" s="25"/>
-      <c r="B54" s="22"/>
-      <c r="C54" s="22"/>
-      <c r="D54" s="22"/>
-      <c r="E54" s="23"/>
-    </row>
-    <row r="55" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A55" s="25"/>
-      <c r="B55" s="22"/>
-      <c r="C55" s="22"/>
-      <c r="D55" s="22"/>
-      <c r="E55" s="23"/>
-    </row>
-    <row r="56" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A56" s="25"/>
-      <c r="B56" s="22"/>
-      <c r="C56" s="22"/>
-      <c r="D56" s="22"/>
-      <c r="E56" s="23"/>
-    </row>
-    <row r="57" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A57" s="25"/>
-      <c r="B57" s="22"/>
-      <c r="C57" s="22"/>
-      <c r="D57" s="22"/>
-      <c r="E57" s="23"/>
-    </row>
-    <row r="58" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A58" s="25"/>
-      <c r="B58" s="22"/>
-      <c r="C58" s="22"/>
-      <c r="D58" s="22"/>
-      <c r="E58" s="23"/>
-    </row>
-    <row r="59" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A59" s="25"/>
-      <c r="B59" s="22"/>
-      <c r="C59" s="22"/>
-      <c r="D59" s="22"/>
-      <c r="E59" s="23"/>
-    </row>
-    <row r="60" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A60" s="25"/>
-      <c r="B60" s="22"/>
-      <c r="C60" s="22"/>
-      <c r="D60" s="22"/>
-      <c r="E60" s="23"/>
-    </row>
-    <row r="61" spans="1:5" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="21" t="s">
+      <c r="B51" s="20"/>
+      <c r="C51" s="20"/>
+      <c r="D51" s="20"/>
+      <c r="E51" s="21"/>
+    </row>
+    <row r="52" spans="1:5" ht="12">
+      <c r="A52" s="24"/>
+      <c r="B52" s="20"/>
+      <c r="C52" s="20"/>
+      <c r="D52" s="20"/>
+      <c r="E52" s="21"/>
+    </row>
+    <row r="53" spans="1:5" ht="12">
+      <c r="A53" s="23"/>
+      <c r="B53" s="20"/>
+      <c r="C53" s="20"/>
+      <c r="D53" s="20"/>
+      <c r="E53" s="21"/>
+    </row>
+    <row r="54" spans="1:5" ht="12">
+      <c r="A54" s="23"/>
+      <c r="B54" s="20"/>
+      <c r="C54" s="20"/>
+      <c r="D54" s="20"/>
+      <c r="E54" s="21"/>
+    </row>
+    <row r="55" spans="1:5" ht="12">
+      <c r="A55" s="23"/>
+      <c r="B55" s="20"/>
+      <c r="C55" s="20"/>
+      <c r="D55" s="20"/>
+      <c r="E55" s="21"/>
+    </row>
+    <row r="56" spans="1:5" ht="12">
+      <c r="A56" s="23"/>
+      <c r="B56" s="20"/>
+      <c r="C56" s="20"/>
+      <c r="D56" s="20"/>
+      <c r="E56" s="21"/>
+    </row>
+    <row r="57" spans="1:5" ht="12">
+      <c r="A57" s="23"/>
+      <c r="B57" s="20"/>
+      <c r="C57" s="20"/>
+      <c r="D57" s="20"/>
+      <c r="E57" s="21"/>
+    </row>
+    <row r="58" spans="1:5" ht="12">
+      <c r="A58" s="23"/>
+      <c r="B58" s="20"/>
+      <c r="C58" s="20"/>
+      <c r="D58" s="20"/>
+      <c r="E58" s="21"/>
+    </row>
+    <row r="59" spans="1:5" ht="12">
+      <c r="A59" s="23"/>
+      <c r="B59" s="20"/>
+      <c r="C59" s="20"/>
+      <c r="D59" s="20"/>
+      <c r="E59" s="21"/>
+    </row>
+    <row r="60" spans="1:5" ht="12">
+      <c r="A60" s="23"/>
+      <c r="B60" s="20"/>
+      <c r="C60" s="20"/>
+      <c r="D60" s="20"/>
+      <c r="E60" s="21"/>
+    </row>
+    <row r="61" spans="1:5" ht="30" customHeight="1">
+      <c r="A61" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="B61" s="20"/>
+      <c r="C61" s="20"/>
+      <c r="D61" s="20"/>
+      <c r="E61" s="21"/>
+    </row>
+    <row r="62" spans="1:5" ht="12" customHeight="1">
+      <c r="A62" s="36" t="s">
+        <v>41</v>
+      </c>
+      <c r="B62" s="37"/>
+      <c r="C62" s="38"/>
+      <c r="D62" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="E62" s="40"/>
+    </row>
+    <row r="63" spans="1:5" ht="12">
+      <c r="A63" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="B63" s="31"/>
+      <c r="C63" s="32"/>
+      <c r="D63" s="31" t="s">
+        <v>43</v>
+      </c>
+      <c r="E63" s="41"/>
+    </row>
+    <row r="64" spans="1:5" ht="12">
+      <c r="A64" s="30"/>
+      <c r="B64" s="31"/>
+      <c r="C64" s="32"/>
+      <c r="D64" s="31"/>
+      <c r="E64" s="41"/>
+    </row>
+    <row r="65" spans="1:5" ht="12">
+      <c r="A65" s="30"/>
+      <c r="B65" s="31"/>
+      <c r="C65" s="32"/>
+      <c r="D65" s="31"/>
+      <c r="E65" s="41"/>
+    </row>
+    <row r="66" spans="1:5" ht="12">
+      <c r="A66" s="30"/>
+      <c r="B66" s="31"/>
+      <c r="C66" s="32"/>
+      <c r="D66" s="31"/>
+      <c r="E66" s="41"/>
+    </row>
+    <row r="67" spans="1:5" ht="12">
+      <c r="A67" s="33"/>
+      <c r="B67" s="34"/>
+      <c r="C67" s="35"/>
+      <c r="D67" s="31"/>
+      <c r="E67" s="41"/>
+    </row>
+    <row r="68" spans="1:5" ht="13" customHeight="1">
+      <c r="A68" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="B68" s="20"/>
+      <c r="C68" s="20"/>
+      <c r="D68" s="20"/>
+      <c r="E68" s="21"/>
+    </row>
+    <row r="69" spans="1:5" ht="12">
+      <c r="A69" s="22"/>
+      <c r="B69" s="20"/>
+      <c r="C69" s="20"/>
+      <c r="D69" s="20"/>
+      <c r="E69" s="21"/>
+    </row>
+    <row r="70" spans="1:5" ht="12">
+      <c r="A70" s="23"/>
+      <c r="B70" s="20"/>
+      <c r="C70" s="20"/>
+      <c r="D70" s="20"/>
+      <c r="E70" s="21"/>
+    </row>
+    <row r="71" spans="1:5" ht="12">
+      <c r="A71" s="23"/>
+      <c r="B71" s="20"/>
+      <c r="C71" s="20"/>
+      <c r="D71" s="20"/>
+      <c r="E71" s="21"/>
+    </row>
+    <row r="72" spans="1:5" ht="12">
+      <c r="A72" s="23"/>
+      <c r="B72" s="20"/>
+      <c r="C72" s="20"/>
+      <c r="D72" s="20"/>
+      <c r="E72" s="21"/>
+    </row>
+    <row r="73" spans="1:5" ht="12">
+      <c r="A73" s="23"/>
+      <c r="B73" s="20"/>
+      <c r="C73" s="20"/>
+      <c r="D73" s="20"/>
+      <c r="E73" s="21"/>
+    </row>
+    <row r="74" spans="1:5" ht="12">
+      <c r="A74" s="23"/>
+      <c r="B74" s="20"/>
+      <c r="C74" s="20"/>
+      <c r="D74" s="20"/>
+      <c r="E74" s="21"/>
+    </row>
+    <row r="75" spans="1:5" ht="12">
+      <c r="A75" s="23"/>
+      <c r="B75" s="20"/>
+      <c r="C75" s="20"/>
+      <c r="D75" s="20"/>
+      <c r="E75" s="21"/>
+    </row>
+    <row r="76" spans="1:5" ht="13" customHeight="1">
+      <c r="A76" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="B76" s="20"/>
+      <c r="C76" s="20"/>
+      <c r="D76" s="20"/>
+      <c r="E76" s="21"/>
+    </row>
+    <row r="77" spans="1:5" ht="12">
+      <c r="A77" s="24"/>
+      <c r="B77" s="20"/>
+      <c r="C77" s="20"/>
+      <c r="D77" s="20"/>
+      <c r="E77" s="21"/>
+    </row>
+    <row r="78" spans="1:5" ht="12">
+      <c r="A78" s="23"/>
+      <c r="B78" s="20"/>
+      <c r="C78" s="20"/>
+      <c r="D78" s="20"/>
+      <c r="E78" s="21"/>
+    </row>
+    <row r="79" spans="1:5" ht="12">
+      <c r="A79" s="23"/>
+      <c r="B79" s="20"/>
+      <c r="C79" s="20"/>
+      <c r="D79" s="20"/>
+      <c r="E79" s="21"/>
+    </row>
+    <row r="80" spans="1:5" s="18" customFormat="1" ht="12">
+      <c r="A80" s="23"/>
+      <c r="B80" s="20"/>
+      <c r="C80" s="20"/>
+      <c r="D80" s="20"/>
+      <c r="E80" s="21"/>
+    </row>
+    <row r="81" spans="1:5" ht="12">
+      <c r="A81" s="23"/>
+      <c r="B81" s="20"/>
+      <c r="C81" s="20"/>
+      <c r="D81" s="20"/>
+      <c r="E81" s="21"/>
+    </row>
+    <row r="82" spans="1:5" ht="12">
+      <c r="A82" s="23"/>
+      <c r="B82" s="20"/>
+      <c r="C82" s="20"/>
+      <c r="D82" s="20"/>
+      <c r="E82" s="21"/>
+    </row>
+    <row r="83" spans="1:5" ht="12">
+      <c r="A83" s="23"/>
+      <c r="B83" s="20"/>
+      <c r="C83" s="20"/>
+      <c r="D83" s="20"/>
+      <c r="E83" s="21"/>
+    </row>
+    <row r="84" spans="1:5" ht="30" customHeight="1">
+      <c r="A84" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="B61" s="22"/>
-      <c r="C61" s="22"/>
-      <c r="D61" s="22"/>
-      <c r="E61" s="23"/>
-    </row>
-    <row r="62" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="38" t="s">
-        <v>41</v>
-      </c>
-      <c r="B62" s="39"/>
-      <c r="C62" s="40"/>
-      <c r="D62" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="E62" s="42"/>
-    </row>
-    <row r="63" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A63" s="32" t="s">
-        <v>58</v>
-      </c>
-      <c r="B63" s="33"/>
-      <c r="C63" s="34"/>
-      <c r="D63" s="33" t="s">
-        <v>43</v>
-      </c>
-      <c r="E63" s="43"/>
-    </row>
-    <row r="64" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A64" s="32"/>
-      <c r="B64" s="33"/>
-      <c r="C64" s="34"/>
-      <c r="D64" s="33"/>
-      <c r="E64" s="43"/>
-    </row>
-    <row r="65" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A65" s="32"/>
-      <c r="B65" s="33"/>
-      <c r="C65" s="34"/>
-      <c r="D65" s="33"/>
-      <c r="E65" s="43"/>
-    </row>
-    <row r="66" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A66" s="32"/>
-      <c r="B66" s="33"/>
-      <c r="C66" s="34"/>
-      <c r="D66" s="33"/>
-      <c r="E66" s="43"/>
-    </row>
-    <row r="67" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A67" s="35"/>
-      <c r="B67" s="36"/>
-      <c r="C67" s="37"/>
-      <c r="D67" s="33"/>
-      <c r="E67" s="43"/>
-    </row>
-    <row r="68" spans="1:5" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="21" t="s">
-        <v>44</v>
-      </c>
-      <c r="B68" s="22"/>
-      <c r="C68" s="22"/>
-      <c r="D68" s="22"/>
-      <c r="E68" s="23"/>
-    </row>
-    <row r="69" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A69" s="24"/>
-      <c r="B69" s="22"/>
-      <c r="C69" s="22"/>
-      <c r="D69" s="22"/>
-      <c r="E69" s="23"/>
-    </row>
-    <row r="70" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A70" s="25"/>
-      <c r="B70" s="22"/>
-      <c r="C70" s="22"/>
-      <c r="D70" s="22"/>
-      <c r="E70" s="23"/>
-    </row>
-    <row r="71" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A71" s="25"/>
-      <c r="B71" s="22"/>
-      <c r="C71" s="22"/>
-      <c r="D71" s="22"/>
-      <c r="E71" s="23"/>
-    </row>
-    <row r="72" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A72" s="25"/>
-      <c r="B72" s="22"/>
-      <c r="C72" s="22"/>
-      <c r="D72" s="22"/>
-      <c r="E72" s="23"/>
-    </row>
-    <row r="73" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A73" s="25"/>
-      <c r="B73" s="22"/>
-      <c r="C73" s="22"/>
-      <c r="D73" s="22"/>
-      <c r="E73" s="23"/>
-    </row>
-    <row r="74" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A74" s="25"/>
-      <c r="B74" s="22"/>
-      <c r="C74" s="22"/>
-      <c r="D74" s="22"/>
-      <c r="E74" s="23"/>
-    </row>
-    <row r="75" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A75" s="25"/>
-      <c r="B75" s="22"/>
-      <c r="C75" s="22"/>
-      <c r="D75" s="22"/>
-      <c r="E75" s="23"/>
-    </row>
-    <row r="76" spans="1:5" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="21" t="s">
-        <v>45</v>
-      </c>
-      <c r="B76" s="22"/>
-      <c r="C76" s="22"/>
-      <c r="D76" s="22"/>
-      <c r="E76" s="23"/>
-    </row>
-    <row r="77" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A77" s="26"/>
-      <c r="B77" s="22"/>
-      <c r="C77" s="22"/>
-      <c r="D77" s="22"/>
-      <c r="E77" s="23"/>
-    </row>
-    <row r="78" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A78" s="25"/>
-      <c r="B78" s="22"/>
-      <c r="C78" s="22"/>
-      <c r="D78" s="22"/>
-      <c r="E78" s="23"/>
-    </row>
-    <row r="79" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A79" s="25"/>
-      <c r="B79" s="22"/>
-      <c r="C79" s="22"/>
-      <c r="D79" s="22"/>
-      <c r="E79" s="23"/>
-    </row>
-    <row r="80" spans="1:5" s="18" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A80" s="25"/>
-      <c r="B80" s="22"/>
-      <c r="C80" s="22"/>
-      <c r="D80" s="22"/>
-      <c r="E80" s="23"/>
-    </row>
-    <row r="81" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A81" s="25"/>
-      <c r="B81" s="22"/>
-      <c r="C81" s="22"/>
-      <c r="D81" s="22"/>
-      <c r="E81" s="23"/>
-    </row>
-    <row r="82" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A82" s="25"/>
-      <c r="B82" s="22"/>
-      <c r="C82" s="22"/>
-      <c r="D82" s="22"/>
-      <c r="E82" s="23"/>
-    </row>
-    <row r="83" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A83" s="25"/>
-      <c r="B83" s="22"/>
-      <c r="C83" s="22"/>
-      <c r="D83" s="22"/>
-      <c r="E83" s="23"/>
-    </row>
-    <row r="84" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A84" s="27" t="s">
-        <v>46</v>
-      </c>
-      <c r="B84" s="22"/>
-      <c r="C84" s="22"/>
-      <c r="D84" s="22"/>
-      <c r="E84" s="23"/>
-    </row>
-    <row r="85" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A85" s="26"/>
-      <c r="B85" s="22"/>
-      <c r="C85" s="22"/>
-      <c r="D85" s="22"/>
-      <c r="E85" s="23"/>
-    </row>
-    <row r="86" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A86" s="25"/>
-      <c r="B86" s="22"/>
-      <c r="C86" s="22"/>
-      <c r="D86" s="22"/>
-      <c r="E86" s="23"/>
-    </row>
-    <row r="87" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A87" s="25"/>
-      <c r="B87" s="22"/>
-      <c r="C87" s="22"/>
-      <c r="D87" s="22"/>
-      <c r="E87" s="23"/>
-    </row>
-    <row r="88" spans="1:5" s="18" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A88" s="25"/>
-      <c r="B88" s="22"/>
-      <c r="C88" s="22"/>
-      <c r="D88" s="22"/>
-      <c r="E88" s="23"/>
-    </row>
-    <row r="89" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A89" s="25"/>
-      <c r="B89" s="22"/>
-      <c r="C89" s="22"/>
-      <c r="D89" s="22"/>
-      <c r="E89" s="23"/>
-    </row>
-    <row r="90" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A90" s="25"/>
-      <c r="B90" s="22"/>
-      <c r="C90" s="22"/>
-      <c r="D90" s="22"/>
-      <c r="E90" s="23"/>
-    </row>
-    <row r="91" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A91" s="25"/>
-      <c r="B91" s="22"/>
-      <c r="C91" s="22"/>
-      <c r="D91" s="22"/>
-      <c r="E91" s="23"/>
-    </row>
-    <row r="92" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B84" s="20"/>
+      <c r="C84" s="20"/>
+      <c r="D84" s="20"/>
+      <c r="E84" s="21"/>
+    </row>
+    <row r="85" spans="1:5" ht="12">
+      <c r="A85" s="24"/>
+      <c r="B85" s="20"/>
+      <c r="C85" s="20"/>
+      <c r="D85" s="20"/>
+      <c r="E85" s="21"/>
+    </row>
+    <row r="86" spans="1:5" ht="12">
+      <c r="A86" s="23"/>
+      <c r="B86" s="20"/>
+      <c r="C86" s="20"/>
+      <c r="D86" s="20"/>
+      <c r="E86" s="21"/>
+    </row>
+    <row r="87" spans="1:5" ht="12">
+      <c r="A87" s="23"/>
+      <c r="B87" s="20"/>
+      <c r="C87" s="20"/>
+      <c r="D87" s="20"/>
+      <c r="E87" s="21"/>
+    </row>
+    <row r="88" spans="1:5" s="18" customFormat="1" ht="12">
+      <c r="A88" s="23"/>
+      <c r="B88" s="20"/>
+      <c r="C88" s="20"/>
+      <c r="D88" s="20"/>
+      <c r="E88" s="21"/>
+    </row>
+    <row r="89" spans="1:5" ht="12">
+      <c r="A89" s="23"/>
+      <c r="B89" s="20"/>
+      <c r="C89" s="20"/>
+      <c r="D89" s="20"/>
+      <c r="E89" s="21"/>
+    </row>
+    <row r="90" spans="1:5" ht="12">
+      <c r="A90" s="23"/>
+      <c r="B90" s="20"/>
+      <c r="C90" s="20"/>
+      <c r="D90" s="20"/>
+      <c r="E90" s="21"/>
+    </row>
+    <row r="91" spans="1:5" ht="12">
+      <c r="A91" s="23"/>
+      <c r="B91" s="20"/>
+      <c r="C91" s="20"/>
+      <c r="D91" s="20"/>
+      <c r="E91" s="21"/>
+    </row>
+    <row r="92" spans="1:5" ht="15" customHeight="1">
       <c r="A92" s="13" t="s">
         <v>28</v>
       </c>
@@ -2127,17 +2103,17 @@
       <c r="D92" s="3"/>
       <c r="E92" s="3"/>
     </row>
-    <row r="93" spans="1:5" ht="4.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A94" s="31" t="s">
+    <row r="93" spans="1:5" ht="4.5" customHeight="1"/>
+    <row r="94" spans="1:5" ht="13">
+      <c r="A94" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="B94" s="29"/>
-      <c r="C94" s="29"/>
-      <c r="D94" s="29"/>
-      <c r="E94" s="29"/>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B94" s="27"/>
+      <c r="C94" s="27"/>
+      <c r="D94" s="27"/>
+      <c r="E94" s="27"/>
+    </row>
+    <row r="95" spans="1:5" ht="13">
       <c r="A95" s="2" t="s">
         <v>30</v>
       </c>
@@ -2145,7 +2121,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:5" ht="13">
       <c r="A96" s="2" t="s">
         <v>32</v>
       </c>
@@ -2153,7 +2129,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:5" ht="13">
       <c r="A97" s="2" t="s">
         <v>34</v>
       </c>
@@ -2161,7 +2137,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="98" spans="1:5" ht="57" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:5" ht="39">
       <c r="A98" s="15" t="s">
         <v>36</v>
       </c>
@@ -2169,116 +2145,93 @@
         <v>37</v>
       </c>
     </row>
-    <row r="99" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="100" spans="1:5" s="18" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A100" s="28" t="s">
-        <v>52</v>
-      </c>
-      <c r="B100" s="28"/>
-      <c r="C100" s="28"/>
-      <c r="D100" s="28"/>
-      <c r="E100" s="28"/>
-    </row>
-    <row r="101" spans="1:5" s="18" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="102" spans="1:5" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A102" s="28" t="s">
-        <v>49</v>
-      </c>
-      <c r="B102" s="29"/>
-      <c r="C102" s="29"/>
-    </row>
-    <row r="103" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="104" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A104" s="28" t="s">
+    <row r="100" spans="1:5" s="18" customFormat="1" ht="13" customHeight="1">
+      <c r="A100" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="B100" s="26"/>
+      <c r="C100" s="26"/>
+      <c r="D100" s="26"/>
+      <c r="E100" s="26"/>
+    </row>
+    <row r="101" spans="1:5" s="18" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="102" spans="1:5" ht="13" customHeight="1">
+      <c r="A102" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="B102" s="27"/>
+      <c r="C102" s="27"/>
+    </row>
+    <row r="104" spans="1:5" ht="30" customHeight="1">
+      <c r="A104" s="26" t="s">
+        <v>56</v>
+      </c>
+      <c r="B104" s="27"/>
+      <c r="C104" s="27"/>
+      <c r="D104" s="27"/>
+      <c r="E104" s="27"/>
+    </row>
+    <row r="106" spans="1:5" ht="30" customHeight="1">
+      <c r="A106" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="B106" s="27"/>
+      <c r="C106" s="27"/>
+      <c r="D106" s="27"/>
+      <c r="E106" s="27"/>
+    </row>
+    <row r="108" spans="1:5" ht="30" customHeight="1">
+      <c r="A108" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="B104" s="29"/>
-      <c r="C104" s="29"/>
-      <c r="D104" s="29"/>
-      <c r="E104" s="29"/>
-    </row>
-    <row r="105" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="106" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A106" s="28" t="s">
-        <v>56</v>
-      </c>
-      <c r="B106" s="29"/>
-      <c r="C106" s="29"/>
-      <c r="D106" s="29"/>
-      <c r="E106" s="29"/>
-    </row>
-    <row r="107" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="108" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A108" s="28" t="s">
-        <v>54</v>
-      </c>
-      <c r="B108" s="29"/>
-      <c r="C108" s="29"/>
-      <c r="D108" s="29"/>
-      <c r="E108" s="29"/>
-    </row>
-    <row r="109" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="110" spans="1:5" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A110" s="28" t="s">
-        <v>57</v>
-      </c>
-      <c r="B110" s="29"/>
-      <c r="C110" s="29"/>
-      <c r="D110" s="29"/>
-      <c r="E110" s="29"/>
-    </row>
-    <row r="111" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="112" spans="1:5" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A112" s="28" t="s">
-        <v>50</v>
-      </c>
-      <c r="B112" s="30"/>
-      <c r="C112" s="30"/>
-      <c r="D112" s="30"/>
-      <c r="E112" s="30"/>
-    </row>
-    <row r="113" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B108" s="27"/>
+      <c r="C108" s="27"/>
+      <c r="D108" s="27"/>
+      <c r="E108" s="27"/>
+    </row>
+    <row r="110" spans="1:5" ht="40" customHeight="1">
+      <c r="A110" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="B110" s="27"/>
+      <c r="C110" s="27"/>
+      <c r="D110" s="27"/>
+      <c r="E110" s="27"/>
+    </row>
+    <row r="112" spans="1:5" ht="40" customHeight="1">
+      <c r="A112" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="B112" s="28"/>
+      <c r="C112" s="28"/>
+      <c r="D112" s="28"/>
+      <c r="E112" s="28"/>
+    </row>
+    <row r="113" spans="1:5" ht="14" customHeight="1">
       <c r="A113" s="16"/>
       <c r="B113" s="17"/>
       <c r="C113" s="17"/>
       <c r="D113" s="17"/>
       <c r="E113" s="17"/>
     </row>
-    <row r="114" spans="1:5" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A114" s="28" t="s">
-        <v>51</v>
-      </c>
-      <c r="B114" s="28"/>
-      <c r="C114" s="28"/>
-      <c r="D114" s="28"/>
-      <c r="E114" s="28"/>
-    </row>
-    <row r="115" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="116" spans="1:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A116" s="28" t="s">
-        <v>53</v>
-      </c>
-      <c r="B116" s="29"/>
-      <c r="C116" s="29"/>
-      <c r="D116" s="29"/>
-      <c r="E116" s="29"/>
-    </row>
-    <row r="117" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="118" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="119" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="120" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="121" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="122" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="123" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="124" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="125" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="126" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="127" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="128" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="129" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="130" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="131" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="132" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="114" spans="1:5" ht="40" customHeight="1">
+      <c r="A114" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="B114" s="26"/>
+      <c r="C114" s="26"/>
+      <c r="D114" s="26"/>
+      <c r="E114" s="26"/>
+    </row>
+    <row r="116" spans="1:5" ht="30.75" customHeight="1">
+      <c r="A116" s="26" t="s">
+        <v>54</v>
+      </c>
+      <c r="B116" s="27"/>
+      <c r="C116" s="27"/>
+      <c r="D116" s="27"/>
+      <c r="E116" s="27"/>
+    </row>
   </sheetData>
   <mergeCells count="62">
     <mergeCell ref="A1:E1"/>
@@ -2346,10 +2299,10 @@
   </mergeCells>
   <phoneticPr fontId="26" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="1" OnePage="0" WScale="0"/>
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
 </worksheet>
@@ -2361,7 +2314,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
   <sheetData/>
   <phoneticPr fontId="26" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2380,7 +2333,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
   <sheetData/>
   <phoneticPr fontId="26" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
updated recommendation and app forms 2
</commit_message>
<xml_diff>
--- a/app/assets/files/NAPI 2013 Application Form.xlsx
+++ b/app/assets/files/NAPI 2013 Application Form.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23416"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr checkCompatibility="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="13940" tabRatio="500"/>
+    <workbookView xWindow="-735" yWindow="-21045" windowWidth="20730" windowHeight="11760" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Application" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
@@ -218,9 +218,6 @@
     <t>1 year</t>
   </si>
   <si>
-    <t>Example:  Experience with vacuum systems</t>
-  </si>
-  <si>
     <t>4. Why should you be accepted into this program? (100 words)</t>
   </si>
   <si>
@@ -331,17 +328,31 @@
     </r>
   </si>
   <si>
-    <t>5. Send the PDF files to internship.naist@gmail.com on or before July 19, 2013 11:59 PM (Philippine standard time) with NAPI2013 Application as the subject line of your email.</t>
-  </si>
-  <si>
-    <t>7. Deadline for the recommendation form is on or before July 19, 2013 11:59 PM (Philippine standard time). Please contact your professors/advisers beforehand about your application. Kindly ask them to send the document directly to internship.naist@gmail.com in PDF format.</t>
+    <t>5. Send the PDF files to internship.naist@gmail.com on or before July 19, 2013 23:59 GMT+8 with NAPI2013 Application as the subject line of your email.</t>
+  </si>
+  <si>
+    <t>7. Deadline for the recommendation form is on or before July 19, 2013 23:59 GMT+8. Please contact your professors/advisers beforehand about your application. Kindly ask them to send the document directly to internship.naist@gmail.com in PDF format.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Example:  Experience with vacuum systems </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>(Kindly delete this when filling the form)</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="31" x14ac:knownFonts="1">
+  <fonts count="32" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -502,6 +513,12 @@
       <u/>
       <sz val="10"/>
       <color theme="11"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
   </fonts>
@@ -909,6 +926,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1017,6 +1036,9 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1026,17 +1048,12 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1045,6 +1062,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1370,46 +1392,48 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E116"/>
+  <dimension ref="A1:F132"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22:E24"/>
+    <sheetView tabSelected="1" showWhiteSpace="0" view="pageLayout" topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="A52" sqref="A52:E60"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14.25" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.25" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="3" width="23" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" customWidth="1"/>
-    <col min="5" max="5" width="9.1640625" customWidth="1"/>
-    <col min="6" max="6" width="2.1640625" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" customWidth="1"/>
+    <col min="6" max="6" width="2.140625" hidden="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A1" s="47" t="s">
+    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-    </row>
-    <row r="3" spans="1:5" ht="13">
-      <c r="A3" s="43" t="s">
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+    </row>
+    <row r="2" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="44"/>
-      <c r="C3" s="44"/>
-      <c r="D3" s="44"/>
-      <c r="E3" s="44"/>
-    </row>
-    <row r="4" spans="1:5" ht="6" customHeight="1">
+      <c r="B3" s="46"/>
+      <c r="C3" s="46"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="46"/>
+    </row>
+    <row r="4" spans="1:5" ht="6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="10"/>
       <c r="B4" s="10"/>
       <c r="C4" s="10"/>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
     </row>
-    <row r="5" spans="1:5" ht="13">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>2</v>
       </c>
@@ -1419,19 +1443,19 @@
       <c r="C5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="59" t="s">
+      <c r="D5" s="61" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="60"/>
-    </row>
-    <row r="6" spans="1:5" ht="30" customHeight="1">
+      <c r="E5" s="57"/>
+    </row>
+    <row r="6" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="11"/>
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
-      <c r="D6" s="23"/>
-      <c r="E6" s="60"/>
-    </row>
-    <row r="7" spans="1:5" ht="13">
+      <c r="D6" s="25"/>
+      <c r="E6" s="57"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>6</v>
       </c>
@@ -1441,130 +1465,130 @@
       <c r="C7" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="23"/>
-      <c r="E7" s="60"/>
-    </row>
-    <row r="8" spans="1:5" ht="30" customHeight="1">
+      <c r="D7" s="25"/>
+      <c r="E7" s="57"/>
+    </row>
+    <row r="8" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="11"/>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
-      <c r="D8" s="23"/>
-      <c r="E8" s="60"/>
-    </row>
-    <row r="9" spans="1:5" ht="13">
-      <c r="A9" s="58" t="s">
+      <c r="D8" s="25"/>
+      <c r="E8" s="57"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="62" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="21"/>
+      <c r="B9" s="23"/>
       <c r="C9" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="23"/>
-      <c r="E9" s="60"/>
-    </row>
-    <row r="10" spans="1:5" ht="30" customHeight="1">
-      <c r="A10" s="57"/>
-      <c r="B10" s="21"/>
+      <c r="D9" s="25"/>
+      <c r="E9" s="57"/>
+    </row>
+    <row r="10" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="60"/>
+      <c r="B10" s="23"/>
       <c r="C10" s="11"/>
-      <c r="D10" s="23"/>
-      <c r="E10" s="60"/>
-    </row>
-    <row r="11" spans="1:5" ht="25" customHeight="1">
+      <c r="D10" s="25"/>
+      <c r="E10" s="57"/>
+    </row>
+    <row r="11" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
     </row>
-    <row r="12" spans="1:5" ht="13">
-      <c r="A12" s="43" t="s">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="45" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="44"/>
-      <c r="C12" s="44"/>
-      <c r="D12" s="44"/>
-      <c r="E12" s="44"/>
-    </row>
-    <row r="13" spans="1:5" ht="6" customHeight="1">
+      <c r="B12" s="46"/>
+      <c r="C12" s="46"/>
+      <c r="D12" s="46"/>
+      <c r="E12" s="46"/>
+    </row>
+    <row r="13" spans="1:5" ht="6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="10"/>
       <c r="B13" s="10"/>
       <c r="C13" s="10"/>
       <c r="D13" s="10"/>
       <c r="E13" s="10"/>
     </row>
-    <row r="14" spans="1:5" ht="30" customHeight="1">
-      <c r="A14" s="54" t="s">
+    <row r="14" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="56" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="21"/>
+      <c r="B14" s="23"/>
       <c r="C14" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="56" t="s">
+      <c r="D14" s="59" t="s">
         <v>14</v>
       </c>
-      <c r="E14" s="60"/>
-    </row>
-    <row r="15" spans="1:5" ht="30" customHeight="1">
-      <c r="A15" s="57"/>
-      <c r="B15" s="21"/>
+      <c r="E14" s="57"/>
+    </row>
+    <row r="15" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="60"/>
+      <c r="B15" s="23"/>
       <c r="C15" s="11"/>
-      <c r="D15" s="49"/>
-      <c r="E15" s="60"/>
-    </row>
-    <row r="16" spans="1:5" ht="13">
-      <c r="A16" s="54" t="s">
+      <c r="D15" s="51"/>
+      <c r="E15" s="57"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="56" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="46"/>
-      <c r="C16" s="21"/>
-      <c r="D16" s="48" t="s">
+      <c r="B16" s="48"/>
+      <c r="C16" s="23"/>
+      <c r="D16" s="50" t="s">
         <v>16</v>
       </c>
-      <c r="E16" s="60"/>
-    </row>
-    <row r="17" spans="1:5" ht="30" customHeight="1">
-      <c r="A17" s="49"/>
-      <c r="B17" s="46"/>
-      <c r="C17" s="21"/>
-      <c r="D17" s="49"/>
-      <c r="E17" s="60"/>
-    </row>
-    <row r="18" spans="1:5" ht="30" customHeight="1">
-      <c r="A18" s="55" t="s">
+      <c r="E16" s="57"/>
+    </row>
+    <row r="17" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="51"/>
+      <c r="B17" s="48"/>
+      <c r="C17" s="23"/>
+      <c r="D17" s="51"/>
+      <c r="E17" s="57"/>
+    </row>
+    <row r="18" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="B18" s="20"/>
-      <c r="C18" s="20"/>
-      <c r="D18" s="20"/>
-      <c r="E18" s="60"/>
-    </row>
-    <row r="19" spans="1:5" ht="30" customHeight="1">
-      <c r="A19" s="49"/>
-      <c r="B19" s="46"/>
-      <c r="C19" s="46"/>
-      <c r="D19" s="46"/>
-      <c r="E19" s="20"/>
-    </row>
-    <row r="20" spans="1:5" ht="13">
-      <c r="A20" s="50" t="s">
+      <c r="B18" s="22"/>
+      <c r="C18" s="22"/>
+      <c r="D18" s="22"/>
+      <c r="E18" s="57"/>
+    </row>
+    <row r="19" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="51"/>
+      <c r="B19" s="48"/>
+      <c r="C19" s="48"/>
+      <c r="D19" s="48"/>
+      <c r="E19" s="22"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="52" t="s">
         <v>17</v>
       </c>
-      <c r="B20" s="20"/>
-      <c r="C20" s="20"/>
-      <c r="D20" s="20"/>
-      <c r="E20" s="21"/>
-    </row>
-    <row r="21" spans="1:5" ht="30" customHeight="1">
-      <c r="A21" s="51" t="s">
-        <v>49</v>
-      </c>
-      <c r="B21" s="52"/>
-      <c r="C21" s="52"/>
-      <c r="D21" s="52"/>
-      <c r="E21" s="53"/>
-    </row>
-    <row r="22" spans="1:5" ht="30" customHeight="1">
+      <c r="B20" s="22"/>
+      <c r="C20" s="22"/>
+      <c r="D20" s="22"/>
+      <c r="E20" s="23"/>
+    </row>
+    <row r="21" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="53" t="s">
+        <v>48</v>
+      </c>
+      <c r="B21" s="54"/>
+      <c r="C21" s="54"/>
+      <c r="D21" s="54"/>
+      <c r="E21" s="55"/>
+    </row>
+    <row r="22" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="8" t="s">
         <v>18</v>
       </c>
@@ -1573,9 +1597,9 @@
       </c>
       <c r="C22" s="7"/>
       <c r="D22" s="7"/>
-      <c r="E22" s="61"/>
-    </row>
-    <row r="23" spans="1:5" ht="30" customHeight="1">
+      <c r="E22" s="19"/>
+    </row>
+    <row r="23" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="8" t="s">
         <v>20</v>
       </c>
@@ -1584,517 +1608,517 @@
       </c>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
-      <c r="E23" s="61"/>
-    </row>
-    <row r="24" spans="1:5" ht="13">
+      <c r="E23" s="19"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="12"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
-      <c r="E24" s="62"/>
-    </row>
-    <row r="25" spans="1:5" ht="25" customHeight="1">
+      <c r="E24" s="20"/>
+    </row>
+    <row r="25" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
     </row>
-    <row r="26" spans="1:5" ht="13">
-      <c r="A26" s="43" t="s">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" s="45" t="s">
         <v>21</v>
       </c>
-      <c r="B26" s="44"/>
-      <c r="C26" s="44"/>
-      <c r="D26" s="44"/>
-      <c r="E26" s="44"/>
-    </row>
-    <row r="27" spans="1:5" ht="4.5" customHeight="1">
+      <c r="B26" s="46"/>
+      <c r="C26" s="46"/>
+      <c r="D26" s="46"/>
+      <c r="E26" s="46"/>
+    </row>
+    <row r="27" spans="1:5" ht="4.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="10"/>
       <c r="B27" s="10"/>
       <c r="C27" s="10"/>
       <c r="D27" s="10"/>
       <c r="E27" s="10"/>
     </row>
-    <row r="28" spans="1:5" ht="13">
-      <c r="A28" s="48" t="s">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" s="50" t="s">
         <v>22</v>
       </c>
-      <c r="B28" s="20"/>
-      <c r="C28" s="20"/>
-      <c r="D28" s="20"/>
-      <c r="E28" s="21"/>
-    </row>
-    <row r="29" spans="1:5" ht="22.5" customHeight="1">
-      <c r="A29" s="24"/>
-      <c r="B29" s="20"/>
-      <c r="C29" s="20"/>
-      <c r="D29" s="20"/>
-      <c r="E29" s="21"/>
-    </row>
-    <row r="30" spans="1:5" ht="13">
-      <c r="A30" s="48" t="s">
+      <c r="B28" s="22"/>
+      <c r="C28" s="22"/>
+      <c r="D28" s="22"/>
+      <c r="E28" s="23"/>
+    </row>
+    <row r="29" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="26"/>
+      <c r="B29" s="22"/>
+      <c r="C29" s="22"/>
+      <c r="D29" s="22"/>
+      <c r="E29" s="23"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" s="50" t="s">
         <v>23</v>
       </c>
-      <c r="B30" s="20"/>
-      <c r="C30" s="20"/>
-      <c r="D30" s="20"/>
-      <c r="E30" s="21"/>
-    </row>
-    <row r="31" spans="1:5" ht="22.5" customHeight="1">
-      <c r="A31" s="24"/>
-      <c r="B31" s="20"/>
-      <c r="C31" s="20"/>
-      <c r="D31" s="20"/>
-      <c r="E31" s="21"/>
-    </row>
-    <row r="32" spans="1:5" ht="13">
-      <c r="A32" s="48" t="s">
+      <c r="B30" s="22"/>
+      <c r="C30" s="22"/>
+      <c r="D30" s="22"/>
+      <c r="E30" s="23"/>
+    </row>
+    <row r="31" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="26"/>
+      <c r="B31" s="22"/>
+      <c r="C31" s="22"/>
+      <c r="D31" s="22"/>
+      <c r="E31" s="23"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" s="50" t="s">
         <v>24</v>
       </c>
-      <c r="B32" s="20"/>
-      <c r="C32" s="20"/>
-      <c r="D32" s="20"/>
-      <c r="E32" s="21"/>
-    </row>
-    <row r="33" spans="1:5" ht="22.5" customHeight="1">
-      <c r="A33" s="24"/>
-      <c r="B33" s="20"/>
-      <c r="C33" s="20"/>
-      <c r="D33" s="20"/>
-      <c r="E33" s="21"/>
-    </row>
-    <row r="34" spans="1:5" ht="15" customHeight="1">
+      <c r="B32" s="22"/>
+      <c r="C32" s="22"/>
+      <c r="D32" s="22"/>
+      <c r="E32" s="23"/>
+    </row>
+    <row r="33" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="26"/>
+      <c r="B33" s="22"/>
+      <c r="C33" s="22"/>
+      <c r="D33" s="22"/>
+      <c r="E33" s="23"/>
+    </row>
+    <row r="34" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
       <c r="E34" s="3"/>
     </row>
-    <row r="35" spans="1:5" ht="12">
-      <c r="A35" s="42" t="s">
+    <row r="35" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A35" s="44" t="s">
         <v>25</v>
       </c>
-      <c r="B35" s="27"/>
-      <c r="C35" s="27"/>
-      <c r="D35" s="27"/>
-      <c r="E35" s="27"/>
-    </row>
-    <row r="36" spans="1:5" ht="22.5" customHeight="1">
+      <c r="B35" s="29"/>
+      <c r="C35" s="29"/>
+      <c r="D35" s="29"/>
+      <c r="E35" s="29"/>
+    </row>
+    <row r="36" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B36" s="43"/>
-      <c r="C36" s="44"/>
-    </row>
-    <row r="37" spans="1:5" ht="22.5" customHeight="1">
+      <c r="B36" s="45"/>
+      <c r="C36" s="46"/>
+    </row>
+    <row r="37" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B37" s="45"/>
-      <c r="C37" s="46"/>
-    </row>
-    <row r="38" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A38" s="47" t="s">
+      <c r="B37" s="47"/>
+      <c r="C37" s="48"/>
+    </row>
+    <row r="38" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="B38" s="27"/>
-      <c r="C38" s="27"/>
-      <c r="D38" s="27"/>
-      <c r="E38" s="27"/>
-    </row>
-    <row r="39" spans="1:5" ht="12">
+      <c r="B38" s="29"/>
+      <c r="C38" s="29"/>
+      <c r="D38" s="29"/>
+      <c r="E38" s="29"/>
+    </row>
+    <row r="39" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A39" s="9"/>
       <c r="B39" s="9"/>
       <c r="C39" s="9"/>
       <c r="D39" s="9"/>
       <c r="E39" s="9"/>
     </row>
-    <row r="40" spans="1:5" ht="30" customHeight="1">
-      <c r="A40" s="25" t="s">
+    <row r="40" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="B40" s="20"/>
-      <c r="C40" s="20"/>
-      <c r="D40" s="20"/>
-      <c r="E40" s="21"/>
-    </row>
-    <row r="41" spans="1:5" ht="12">
-      <c r="A41" s="24"/>
-      <c r="B41" s="20"/>
-      <c r="C41" s="20"/>
-      <c r="D41" s="20"/>
-      <c r="E41" s="21"/>
-    </row>
-    <row r="42" spans="1:5" ht="12">
-      <c r="A42" s="23"/>
-      <c r="B42" s="20"/>
-      <c r="C42" s="20"/>
-      <c r="D42" s="20"/>
-      <c r="E42" s="21"/>
-    </row>
-    <row r="43" spans="1:5" ht="12">
-      <c r="A43" s="23"/>
-      <c r="B43" s="20"/>
-      <c r="C43" s="20"/>
-      <c r="D43" s="20"/>
-      <c r="E43" s="21"/>
-    </row>
-    <row r="44" spans="1:5" s="18" customFormat="1" ht="12">
-      <c r="A44" s="23"/>
-      <c r="B44" s="20"/>
-      <c r="C44" s="20"/>
-      <c r="D44" s="20"/>
-      <c r="E44" s="21"/>
-    </row>
-    <row r="45" spans="1:5" s="18" customFormat="1" ht="12">
-      <c r="A45" s="23"/>
-      <c r="B45" s="20"/>
-      <c r="C45" s="20"/>
-      <c r="D45" s="20"/>
-      <c r="E45" s="21"/>
-    </row>
-    <row r="46" spans="1:5" ht="12">
-      <c r="A46" s="23"/>
-      <c r="B46" s="20"/>
-      <c r="C46" s="20"/>
-      <c r="D46" s="20"/>
-      <c r="E46" s="21"/>
-    </row>
-    <row r="47" spans="1:5" ht="12">
-      <c r="A47" s="23"/>
-      <c r="B47" s="20"/>
-      <c r="C47" s="20"/>
-      <c r="D47" s="20"/>
-      <c r="E47" s="21"/>
-    </row>
-    <row r="48" spans="1:5" ht="12">
-      <c r="A48" s="23"/>
-      <c r="B48" s="20"/>
-      <c r="C48" s="20"/>
-      <c r="D48" s="20"/>
-      <c r="E48" s="21"/>
-    </row>
-    <row r="49" spans="1:5" ht="12">
-      <c r="A49" s="23"/>
-      <c r="B49" s="20"/>
-      <c r="C49" s="20"/>
-      <c r="D49" s="20"/>
-      <c r="E49" s="21"/>
-    </row>
-    <row r="50" spans="1:5" ht="12">
-      <c r="A50" s="23"/>
-      <c r="B50" s="20"/>
-      <c r="C50" s="20"/>
-      <c r="D50" s="20"/>
-      <c r="E50" s="21"/>
-    </row>
-    <row r="51" spans="1:5" ht="30" customHeight="1">
-      <c r="A51" s="19" t="s">
+      <c r="B40" s="22"/>
+      <c r="C40" s="22"/>
+      <c r="D40" s="22"/>
+      <c r="E40" s="23"/>
+    </row>
+    <row r="41" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A41" s="26"/>
+      <c r="B41" s="22"/>
+      <c r="C41" s="22"/>
+      <c r="D41" s="22"/>
+      <c r="E41" s="23"/>
+    </row>
+    <row r="42" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A42" s="25"/>
+      <c r="B42" s="22"/>
+      <c r="C42" s="22"/>
+      <c r="D42" s="22"/>
+      <c r="E42" s="23"/>
+    </row>
+    <row r="43" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A43" s="25"/>
+      <c r="B43" s="22"/>
+      <c r="C43" s="22"/>
+      <c r="D43" s="22"/>
+      <c r="E43" s="23"/>
+    </row>
+    <row r="44" spans="1:5" s="18" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A44" s="25"/>
+      <c r="B44" s="22"/>
+      <c r="C44" s="22"/>
+      <c r="D44" s="22"/>
+      <c r="E44" s="23"/>
+    </row>
+    <row r="45" spans="1:5" s="18" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A45" s="25"/>
+      <c r="B45" s="22"/>
+      <c r="C45" s="22"/>
+      <c r="D45" s="22"/>
+      <c r="E45" s="23"/>
+    </row>
+    <row r="46" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A46" s="25"/>
+      <c r="B46" s="22"/>
+      <c r="C46" s="22"/>
+      <c r="D46" s="22"/>
+      <c r="E46" s="23"/>
+    </row>
+    <row r="47" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A47" s="25"/>
+      <c r="B47" s="22"/>
+      <c r="C47" s="22"/>
+      <c r="D47" s="22"/>
+      <c r="E47" s="23"/>
+    </row>
+    <row r="48" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A48" s="25"/>
+      <c r="B48" s="22"/>
+      <c r="C48" s="22"/>
+      <c r="D48" s="22"/>
+      <c r="E48" s="23"/>
+    </row>
+    <row r="49" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A49" s="25"/>
+      <c r="B49" s="22"/>
+      <c r="C49" s="22"/>
+      <c r="D49" s="22"/>
+      <c r="E49" s="23"/>
+    </row>
+    <row r="50" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A50" s="25"/>
+      <c r="B50" s="22"/>
+      <c r="C50" s="22"/>
+      <c r="D50" s="22"/>
+      <c r="E50" s="23"/>
+    </row>
+    <row r="51" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="B51" s="20"/>
-      <c r="C51" s="20"/>
-      <c r="D51" s="20"/>
-      <c r="E51" s="21"/>
-    </row>
-    <row r="52" spans="1:5" ht="12">
-      <c r="A52" s="24"/>
-      <c r="B52" s="20"/>
-      <c r="C52" s="20"/>
-      <c r="D52" s="20"/>
-      <c r="E52" s="21"/>
-    </row>
-    <row r="53" spans="1:5" ht="12">
-      <c r="A53" s="23"/>
-      <c r="B53" s="20"/>
-      <c r="C53" s="20"/>
-      <c r="D53" s="20"/>
-      <c r="E53" s="21"/>
-    </row>
-    <row r="54" spans="1:5" ht="12">
-      <c r="A54" s="23"/>
-      <c r="B54" s="20"/>
-      <c r="C54" s="20"/>
-      <c r="D54" s="20"/>
-      <c r="E54" s="21"/>
-    </row>
-    <row r="55" spans="1:5" ht="12">
-      <c r="A55" s="23"/>
-      <c r="B55" s="20"/>
-      <c r="C55" s="20"/>
-      <c r="D55" s="20"/>
-      <c r="E55" s="21"/>
-    </row>
-    <row r="56" spans="1:5" ht="12">
-      <c r="A56" s="23"/>
-      <c r="B56" s="20"/>
-      <c r="C56" s="20"/>
-      <c r="D56" s="20"/>
-      <c r="E56" s="21"/>
-    </row>
-    <row r="57" spans="1:5" ht="12">
-      <c r="A57" s="23"/>
-      <c r="B57" s="20"/>
-      <c r="C57" s="20"/>
-      <c r="D57" s="20"/>
-      <c r="E57" s="21"/>
-    </row>
-    <row r="58" spans="1:5" ht="12">
-      <c r="A58" s="23"/>
-      <c r="B58" s="20"/>
-      <c r="C58" s="20"/>
-      <c r="D58" s="20"/>
-      <c r="E58" s="21"/>
-    </row>
-    <row r="59" spans="1:5" ht="12">
-      <c r="A59" s="23"/>
-      <c r="B59" s="20"/>
-      <c r="C59" s="20"/>
-      <c r="D59" s="20"/>
-      <c r="E59" s="21"/>
-    </row>
-    <row r="60" spans="1:5" ht="12">
-      <c r="A60" s="23"/>
-      <c r="B60" s="20"/>
-      <c r="C60" s="20"/>
-      <c r="D60" s="20"/>
-      <c r="E60" s="21"/>
-    </row>
-    <row r="61" spans="1:5" ht="30" customHeight="1">
-      <c r="A61" s="19" t="s">
-        <v>48</v>
-      </c>
-      <c r="B61" s="20"/>
-      <c r="C61" s="20"/>
-      <c r="D61" s="20"/>
-      <c r="E61" s="21"/>
-    </row>
-    <row r="62" spans="1:5" ht="12" customHeight="1">
-      <c r="A62" s="36" t="s">
+      <c r="B51" s="22"/>
+      <c r="C51" s="22"/>
+      <c r="D51" s="22"/>
+      <c r="E51" s="23"/>
+    </row>
+    <row r="52" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A52" s="26"/>
+      <c r="B52" s="22"/>
+      <c r="C52" s="22"/>
+      <c r="D52" s="22"/>
+      <c r="E52" s="23"/>
+    </row>
+    <row r="53" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A53" s="25"/>
+      <c r="B53" s="22"/>
+      <c r="C53" s="22"/>
+      <c r="D53" s="22"/>
+      <c r="E53" s="23"/>
+    </row>
+    <row r="54" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A54" s="25"/>
+      <c r="B54" s="22"/>
+      <c r="C54" s="22"/>
+      <c r="D54" s="22"/>
+      <c r="E54" s="23"/>
+    </row>
+    <row r="55" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A55" s="25"/>
+      <c r="B55" s="22"/>
+      <c r="C55" s="22"/>
+      <c r="D55" s="22"/>
+      <c r="E55" s="23"/>
+    </row>
+    <row r="56" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A56" s="25"/>
+      <c r="B56" s="22"/>
+      <c r="C56" s="22"/>
+      <c r="D56" s="22"/>
+      <c r="E56" s="23"/>
+    </row>
+    <row r="57" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A57" s="25"/>
+      <c r="B57" s="22"/>
+      <c r="C57" s="22"/>
+      <c r="D57" s="22"/>
+      <c r="E57" s="23"/>
+    </row>
+    <row r="58" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A58" s="25"/>
+      <c r="B58" s="22"/>
+      <c r="C58" s="22"/>
+      <c r="D58" s="22"/>
+      <c r="E58" s="23"/>
+    </row>
+    <row r="59" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A59" s="25"/>
+      <c r="B59" s="22"/>
+      <c r="C59" s="22"/>
+      <c r="D59" s="22"/>
+      <c r="E59" s="23"/>
+    </row>
+    <row r="60" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A60" s="25"/>
+      <c r="B60" s="22"/>
+      <c r="C60" s="22"/>
+      <c r="D60" s="22"/>
+      <c r="E60" s="23"/>
+    </row>
+    <row r="61" spans="1:5" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="B61" s="22"/>
+      <c r="C61" s="22"/>
+      <c r="D61" s="22"/>
+      <c r="E61" s="23"/>
+    </row>
+    <row r="62" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="38" t="s">
         <v>41</v>
       </c>
-      <c r="B62" s="37"/>
-      <c r="C62" s="38"/>
-      <c r="D62" s="39" t="s">
+      <c r="B62" s="39"/>
+      <c r="C62" s="40"/>
+      <c r="D62" s="41" t="s">
         <v>42</v>
       </c>
-      <c r="E62" s="40"/>
-    </row>
-    <row r="63" spans="1:5" ht="12">
-      <c r="A63" s="30" t="s">
+      <c r="E62" s="42"/>
+    </row>
+    <row r="63" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A63" s="32" t="s">
+        <v>58</v>
+      </c>
+      <c r="B63" s="33"/>
+      <c r="C63" s="34"/>
+      <c r="D63" s="33" t="s">
+        <v>43</v>
+      </c>
+      <c r="E63" s="43"/>
+    </row>
+    <row r="64" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A64" s="32"/>
+      <c r="B64" s="33"/>
+      <c r="C64" s="34"/>
+      <c r="D64" s="33"/>
+      <c r="E64" s="43"/>
+    </row>
+    <row r="65" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A65" s="32"/>
+      <c r="B65" s="33"/>
+      <c r="C65" s="34"/>
+      <c r="D65" s="33"/>
+      <c r="E65" s="43"/>
+    </row>
+    <row r="66" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A66" s="32"/>
+      <c r="B66" s="33"/>
+      <c r="C66" s="34"/>
+      <c r="D66" s="33"/>
+      <c r="E66" s="43"/>
+    </row>
+    <row r="67" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A67" s="35"/>
+      <c r="B67" s="36"/>
+      <c r="C67" s="37"/>
+      <c r="D67" s="33"/>
+      <c r="E67" s="43"/>
+    </row>
+    <row r="68" spans="1:5" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A68" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="B63" s="31"/>
-      <c r="C63" s="32"/>
-      <c r="D63" s="31" t="s">
-        <v>43</v>
-      </c>
-      <c r="E63" s="41"/>
-    </row>
-    <row r="64" spans="1:5" ht="12">
-      <c r="A64" s="30"/>
-      <c r="B64" s="31"/>
-      <c r="C64" s="32"/>
-      <c r="D64" s="31"/>
-      <c r="E64" s="41"/>
-    </row>
-    <row r="65" spans="1:5" ht="12">
-      <c r="A65" s="30"/>
-      <c r="B65" s="31"/>
-      <c r="C65" s="32"/>
-      <c r="D65" s="31"/>
-      <c r="E65" s="41"/>
-    </row>
-    <row r="66" spans="1:5" ht="12">
-      <c r="A66" s="30"/>
-      <c r="B66" s="31"/>
-      <c r="C66" s="32"/>
-      <c r="D66" s="31"/>
-      <c r="E66" s="41"/>
-    </row>
-    <row r="67" spans="1:5" ht="12">
-      <c r="A67" s="33"/>
-      <c r="B67" s="34"/>
-      <c r="C67" s="35"/>
-      <c r="D67" s="31"/>
-      <c r="E67" s="41"/>
-    </row>
-    <row r="68" spans="1:5" ht="13" customHeight="1">
-      <c r="A68" s="19" t="s">
+      <c r="B68" s="22"/>
+      <c r="C68" s="22"/>
+      <c r="D68" s="22"/>
+      <c r="E68" s="23"/>
+    </row>
+    <row r="69" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A69" s="24"/>
+      <c r="B69" s="22"/>
+      <c r="C69" s="22"/>
+      <c r="D69" s="22"/>
+      <c r="E69" s="23"/>
+    </row>
+    <row r="70" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A70" s="25"/>
+      <c r="B70" s="22"/>
+      <c r="C70" s="22"/>
+      <c r="D70" s="22"/>
+      <c r="E70" s="23"/>
+    </row>
+    <row r="71" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A71" s="25"/>
+      <c r="B71" s="22"/>
+      <c r="C71" s="22"/>
+      <c r="D71" s="22"/>
+      <c r="E71" s="23"/>
+    </row>
+    <row r="72" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A72" s="25"/>
+      <c r="B72" s="22"/>
+      <c r="C72" s="22"/>
+      <c r="D72" s="22"/>
+      <c r="E72" s="23"/>
+    </row>
+    <row r="73" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A73" s="25"/>
+      <c r="B73" s="22"/>
+      <c r="C73" s="22"/>
+      <c r="D73" s="22"/>
+      <c r="E73" s="23"/>
+    </row>
+    <row r="74" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A74" s="25"/>
+      <c r="B74" s="22"/>
+      <c r="C74" s="22"/>
+      <c r="D74" s="22"/>
+      <c r="E74" s="23"/>
+    </row>
+    <row r="75" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A75" s="25"/>
+      <c r="B75" s="22"/>
+      <c r="C75" s="22"/>
+      <c r="D75" s="22"/>
+      <c r="E75" s="23"/>
+    </row>
+    <row r="76" spans="1:5" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A76" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="B68" s="20"/>
-      <c r="C68" s="20"/>
-      <c r="D68" s="20"/>
-      <c r="E68" s="21"/>
-    </row>
-    <row r="69" spans="1:5" ht="12">
-      <c r="A69" s="22"/>
-      <c r="B69" s="20"/>
-      <c r="C69" s="20"/>
-      <c r="D69" s="20"/>
-      <c r="E69" s="21"/>
-    </row>
-    <row r="70" spans="1:5" ht="12">
-      <c r="A70" s="23"/>
-      <c r="B70" s="20"/>
-      <c r="C70" s="20"/>
-      <c r="D70" s="20"/>
-      <c r="E70" s="21"/>
-    </row>
-    <row r="71" spans="1:5" ht="12">
-      <c r="A71" s="23"/>
-      <c r="B71" s="20"/>
-      <c r="C71" s="20"/>
-      <c r="D71" s="20"/>
-      <c r="E71" s="21"/>
-    </row>
-    <row r="72" spans="1:5" ht="12">
-      <c r="A72" s="23"/>
-      <c r="B72" s="20"/>
-      <c r="C72" s="20"/>
-      <c r="D72" s="20"/>
-      <c r="E72" s="21"/>
-    </row>
-    <row r="73" spans="1:5" ht="12">
-      <c r="A73" s="23"/>
-      <c r="B73" s="20"/>
-      <c r="C73" s="20"/>
-      <c r="D73" s="20"/>
-      <c r="E73" s="21"/>
-    </row>
-    <row r="74" spans="1:5" ht="12">
-      <c r="A74" s="23"/>
-      <c r="B74" s="20"/>
-      <c r="C74" s="20"/>
-      <c r="D74" s="20"/>
-      <c r="E74" s="21"/>
-    </row>
-    <row r="75" spans="1:5" ht="12">
-      <c r="A75" s="23"/>
-      <c r="B75" s="20"/>
-      <c r="C75" s="20"/>
-      <c r="D75" s="20"/>
-      <c r="E75" s="21"/>
-    </row>
-    <row r="76" spans="1:5" ht="13" customHeight="1">
-      <c r="A76" s="19" t="s">
+      <c r="B76" s="22"/>
+      <c r="C76" s="22"/>
+      <c r="D76" s="22"/>
+      <c r="E76" s="23"/>
+    </row>
+    <row r="77" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A77" s="26"/>
+      <c r="B77" s="22"/>
+      <c r="C77" s="22"/>
+      <c r="D77" s="22"/>
+      <c r="E77" s="23"/>
+    </row>
+    <row r="78" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A78" s="25"/>
+      <c r="B78" s="22"/>
+      <c r="C78" s="22"/>
+      <c r="D78" s="22"/>
+      <c r="E78" s="23"/>
+    </row>
+    <row r="79" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A79" s="25"/>
+      <c r="B79" s="22"/>
+      <c r="C79" s="22"/>
+      <c r="D79" s="22"/>
+      <c r="E79" s="23"/>
+    </row>
+    <row r="80" spans="1:5" s="18" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A80" s="25"/>
+      <c r="B80" s="22"/>
+      <c r="C80" s="22"/>
+      <c r="D80" s="22"/>
+      <c r="E80" s="23"/>
+    </row>
+    <row r="81" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A81" s="25"/>
+      <c r="B81" s="22"/>
+      <c r="C81" s="22"/>
+      <c r="D81" s="22"/>
+      <c r="E81" s="23"/>
+    </row>
+    <row r="82" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A82" s="25"/>
+      <c r="B82" s="22"/>
+      <c r="C82" s="22"/>
+      <c r="D82" s="22"/>
+      <c r="E82" s="23"/>
+    </row>
+    <row r="83" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A83" s="25"/>
+      <c r="B83" s="22"/>
+      <c r="C83" s="22"/>
+      <c r="D83" s="22"/>
+      <c r="E83" s="23"/>
+    </row>
+    <row r="84" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A84" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="B76" s="20"/>
-      <c r="C76" s="20"/>
-      <c r="D76" s="20"/>
-      <c r="E76" s="21"/>
-    </row>
-    <row r="77" spans="1:5" ht="12">
-      <c r="A77" s="24"/>
-      <c r="B77" s="20"/>
-      <c r="C77" s="20"/>
-      <c r="D77" s="20"/>
-      <c r="E77" s="21"/>
-    </row>
-    <row r="78" spans="1:5" ht="12">
-      <c r="A78" s="23"/>
-      <c r="B78" s="20"/>
-      <c r="C78" s="20"/>
-      <c r="D78" s="20"/>
-      <c r="E78" s="21"/>
-    </row>
-    <row r="79" spans="1:5" ht="12">
-      <c r="A79" s="23"/>
-      <c r="B79" s="20"/>
-      <c r="C79" s="20"/>
-      <c r="D79" s="20"/>
-      <c r="E79" s="21"/>
-    </row>
-    <row r="80" spans="1:5" s="18" customFormat="1" ht="12">
-      <c r="A80" s="23"/>
-      <c r="B80" s="20"/>
-      <c r="C80" s="20"/>
-      <c r="D80" s="20"/>
-      <c r="E80" s="21"/>
-    </row>
-    <row r="81" spans="1:5" ht="12">
-      <c r="A81" s="23"/>
-      <c r="B81" s="20"/>
-      <c r="C81" s="20"/>
-      <c r="D81" s="20"/>
-      <c r="E81" s="21"/>
-    </row>
-    <row r="82" spans="1:5" ht="12">
-      <c r="A82" s="23"/>
-      <c r="B82" s="20"/>
-      <c r="C82" s="20"/>
-      <c r="D82" s="20"/>
-      <c r="E82" s="21"/>
-    </row>
-    <row r="83" spans="1:5" ht="12">
-      <c r="A83" s="23"/>
-      <c r="B83" s="20"/>
-      <c r="C83" s="20"/>
-      <c r="D83" s="20"/>
-      <c r="E83" s="21"/>
-    </row>
-    <row r="84" spans="1:5" ht="30" customHeight="1">
-      <c r="A84" s="25" t="s">
-        <v>47</v>
-      </c>
-      <c r="B84" s="20"/>
-      <c r="C84" s="20"/>
-      <c r="D84" s="20"/>
-      <c r="E84" s="21"/>
-    </row>
-    <row r="85" spans="1:5" ht="12">
-      <c r="A85" s="24"/>
-      <c r="B85" s="20"/>
-      <c r="C85" s="20"/>
-      <c r="D85" s="20"/>
-      <c r="E85" s="21"/>
-    </row>
-    <row r="86" spans="1:5" ht="12">
-      <c r="A86" s="23"/>
-      <c r="B86" s="20"/>
-      <c r="C86" s="20"/>
-      <c r="D86" s="20"/>
-      <c r="E86" s="21"/>
-    </row>
-    <row r="87" spans="1:5" ht="12">
-      <c r="A87" s="23"/>
-      <c r="B87" s="20"/>
-      <c r="C87" s="20"/>
-      <c r="D87" s="20"/>
-      <c r="E87" s="21"/>
-    </row>
-    <row r="88" spans="1:5" s="18" customFormat="1" ht="12">
-      <c r="A88" s="23"/>
-      <c r="B88" s="20"/>
-      <c r="C88" s="20"/>
-      <c r="D88" s="20"/>
-      <c r="E88" s="21"/>
-    </row>
-    <row r="89" spans="1:5" ht="12">
-      <c r="A89" s="23"/>
-      <c r="B89" s="20"/>
-      <c r="C89" s="20"/>
-      <c r="D89" s="20"/>
-      <c r="E89" s="21"/>
-    </row>
-    <row r="90" spans="1:5" ht="12">
-      <c r="A90" s="23"/>
-      <c r="B90" s="20"/>
-      <c r="C90" s="20"/>
-      <c r="D90" s="20"/>
-      <c r="E90" s="21"/>
-    </row>
-    <row r="91" spans="1:5" ht="12">
-      <c r="A91" s="23"/>
-      <c r="B91" s="20"/>
-      <c r="C91" s="20"/>
-      <c r="D91" s="20"/>
-      <c r="E91" s="21"/>
-    </row>
-    <row r="92" spans="1:5" ht="15" customHeight="1">
+      <c r="B84" s="22"/>
+      <c r="C84" s="22"/>
+      <c r="D84" s="22"/>
+      <c r="E84" s="23"/>
+    </row>
+    <row r="85" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A85" s="26"/>
+      <c r="B85" s="22"/>
+      <c r="C85" s="22"/>
+      <c r="D85" s="22"/>
+      <c r="E85" s="23"/>
+    </row>
+    <row r="86" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A86" s="25"/>
+      <c r="B86" s="22"/>
+      <c r="C86" s="22"/>
+      <c r="D86" s="22"/>
+      <c r="E86" s="23"/>
+    </row>
+    <row r="87" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A87" s="25"/>
+      <c r="B87" s="22"/>
+      <c r="C87" s="22"/>
+      <c r="D87" s="22"/>
+      <c r="E87" s="23"/>
+    </row>
+    <row r="88" spans="1:5" s="18" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A88" s="25"/>
+      <c r="B88" s="22"/>
+      <c r="C88" s="22"/>
+      <c r="D88" s="22"/>
+      <c r="E88" s="23"/>
+    </row>
+    <row r="89" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A89" s="25"/>
+      <c r="B89" s="22"/>
+      <c r="C89" s="22"/>
+      <c r="D89" s="22"/>
+      <c r="E89" s="23"/>
+    </row>
+    <row r="90" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A90" s="25"/>
+      <c r="B90" s="22"/>
+      <c r="C90" s="22"/>
+      <c r="D90" s="22"/>
+      <c r="E90" s="23"/>
+    </row>
+    <row r="91" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A91" s="25"/>
+      <c r="B91" s="22"/>
+      <c r="C91" s="22"/>
+      <c r="D91" s="22"/>
+      <c r="E91" s="23"/>
+    </row>
+    <row r="92" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="13" t="s">
         <v>28</v>
       </c>
@@ -2103,17 +2127,17 @@
       <c r="D92" s="3"/>
       <c r="E92" s="3"/>
     </row>
-    <row r="93" spans="1:5" ht="4.5" customHeight="1"/>
-    <row r="94" spans="1:5" ht="13">
-      <c r="A94" s="29" t="s">
+    <row r="93" spans="1:5" ht="4.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A94" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="B94" s="27"/>
-      <c r="C94" s="27"/>
-      <c r="D94" s="27"/>
-      <c r="E94" s="27"/>
-    </row>
-    <row r="95" spans="1:5" ht="13">
+      <c r="B94" s="29"/>
+      <c r="C94" s="29"/>
+      <c r="D94" s="29"/>
+      <c r="E94" s="29"/>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A95" s="2" t="s">
         <v>30</v>
       </c>
@@ -2121,7 +2145,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="96" spans="1:5" ht="13">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A96" s="2" t="s">
         <v>32</v>
       </c>
@@ -2129,7 +2153,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="97" spans="1:5" ht="13">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A97" s="2" t="s">
         <v>34</v>
       </c>
@@ -2137,7 +2161,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="98" spans="1:5" ht="39">
+    <row r="98" spans="1:5" ht="57" x14ac:dyDescent="0.2">
       <c r="A98" s="15" t="s">
         <v>36</v>
       </c>
@@ -2145,93 +2169,116 @@
         <v>37</v>
       </c>
     </row>
-    <row r="100" spans="1:5" s="18" customFormat="1" ht="13" customHeight="1">
-      <c r="A100" s="26" t="s">
-        <v>53</v>
-      </c>
-      <c r="B100" s="26"/>
-      <c r="C100" s="26"/>
-      <c r="D100" s="26"/>
-      <c r="E100" s="26"/>
-    </row>
-    <row r="101" spans="1:5" s="18" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="102" spans="1:5" ht="13" customHeight="1">
-      <c r="A102" s="26" t="s">
+    <row r="99" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="100" spans="1:5" s="18" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A100" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="B100" s="28"/>
+      <c r="C100" s="28"/>
+      <c r="D100" s="28"/>
+      <c r="E100" s="28"/>
+    </row>
+    <row r="101" spans="1:5" s="18" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="102" spans="1:5" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A102" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="B102" s="29"/>
+      <c r="C102" s="29"/>
+    </row>
+    <row r="103" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="104" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A104" s="28" t="s">
+        <v>55</v>
+      </c>
+      <c r="B104" s="29"/>
+      <c r="C104" s="29"/>
+      <c r="D104" s="29"/>
+      <c r="E104" s="29"/>
+    </row>
+    <row r="105" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="106" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A106" s="28" t="s">
+        <v>56</v>
+      </c>
+      <c r="B106" s="29"/>
+      <c r="C106" s="29"/>
+      <c r="D106" s="29"/>
+      <c r="E106" s="29"/>
+    </row>
+    <row r="107" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="108" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A108" s="28" t="s">
+        <v>54</v>
+      </c>
+      <c r="B108" s="29"/>
+      <c r="C108" s="29"/>
+      <c r="D108" s="29"/>
+      <c r="E108" s="29"/>
+    </row>
+    <row r="109" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="110" spans="1:5" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A110" s="28" t="s">
+        <v>57</v>
+      </c>
+      <c r="B110" s="29"/>
+      <c r="C110" s="29"/>
+      <c r="D110" s="29"/>
+      <c r="E110" s="29"/>
+    </row>
+    <row r="111" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="112" spans="1:5" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A112" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="B102" s="27"/>
-      <c r="C102" s="27"/>
-    </row>
-    <row r="104" spans="1:5" ht="30" customHeight="1">
-      <c r="A104" s="26" t="s">
-        <v>56</v>
-      </c>
-      <c r="B104" s="27"/>
-      <c r="C104" s="27"/>
-      <c r="D104" s="27"/>
-      <c r="E104" s="27"/>
-    </row>
-    <row r="106" spans="1:5" ht="30" customHeight="1">
-      <c r="A106" s="26" t="s">
-        <v>57</v>
-      </c>
-      <c r="B106" s="27"/>
-      <c r="C106" s="27"/>
-      <c r="D106" s="27"/>
-      <c r="E106" s="27"/>
-    </row>
-    <row r="108" spans="1:5" ht="30" customHeight="1">
-      <c r="A108" s="26" t="s">
-        <v>55</v>
-      </c>
-      <c r="B108" s="27"/>
-      <c r="C108" s="27"/>
-      <c r="D108" s="27"/>
-      <c r="E108" s="27"/>
-    </row>
-    <row r="110" spans="1:5" ht="40" customHeight="1">
-      <c r="A110" s="26" t="s">
-        <v>58</v>
-      </c>
-      <c r="B110" s="27"/>
-      <c r="C110" s="27"/>
-      <c r="D110" s="27"/>
-      <c r="E110" s="27"/>
-    </row>
-    <row r="112" spans="1:5" ht="40" customHeight="1">
-      <c r="A112" s="26" t="s">
-        <v>51</v>
-      </c>
-      <c r="B112" s="28"/>
-      <c r="C112" s="28"/>
-      <c r="D112" s="28"/>
-      <c r="E112" s="28"/>
-    </row>
-    <row r="113" spans="1:5" ht="14" customHeight="1">
+      <c r="B112" s="30"/>
+      <c r="C112" s="30"/>
+      <c r="D112" s="30"/>
+      <c r="E112" s="30"/>
+    </row>
+    <row r="113" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113" s="16"/>
       <c r="B113" s="17"/>
       <c r="C113" s="17"/>
       <c r="D113" s="17"/>
       <c r="E113" s="17"/>
     </row>
-    <row r="114" spans="1:5" ht="40" customHeight="1">
-      <c r="A114" s="26" t="s">
-        <v>52</v>
-      </c>
-      <c r="B114" s="26"/>
-      <c r="C114" s="26"/>
-      <c r="D114" s="26"/>
-      <c r="E114" s="26"/>
-    </row>
-    <row r="116" spans="1:5" ht="30.75" customHeight="1">
-      <c r="A116" s="26" t="s">
-        <v>54</v>
-      </c>
-      <c r="B116" s="27"/>
-      <c r="C116" s="27"/>
-      <c r="D116" s="27"/>
-      <c r="E116" s="27"/>
-    </row>
+    <row r="114" spans="1:5" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A114" s="28" t="s">
+        <v>51</v>
+      </c>
+      <c r="B114" s="28"/>
+      <c r="C114" s="28"/>
+      <c r="D114" s="28"/>
+      <c r="E114" s="28"/>
+    </row>
+    <row r="115" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="116" spans="1:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A116" s="28" t="s">
+        <v>53</v>
+      </c>
+      <c r="B116" s="29"/>
+      <c r="C116" s="29"/>
+      <c r="D116" s="29"/>
+      <c r="E116" s="29"/>
+    </row>
+    <row r="117" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="118" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="119" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="120" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="121" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="122" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="123" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="124" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="125" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="126" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="127" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="128" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="129" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="130" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="131" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="132" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="62">
     <mergeCell ref="A1:E1"/>
@@ -2299,10 +2346,10 @@
   </mergeCells>
   <phoneticPr fontId="26" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+      <mx:PLV Mode="1" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
 </worksheet>
@@ -2314,7 +2361,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <phoneticPr fontId="26" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2333,7 +2380,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <phoneticPr fontId="26" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>